<commit_message>
Item System and Balance Work
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -265,13 +265,52 @@
   </si>
   <si>
     <t>item_avalore_gauntlets</t>
+  </si>
+  <si>
+    <t>item_recipe_avalore_philosophers_stone</t>
+  </si>
+  <si>
+    <t>item_avalore_philosophers_stone</t>
+  </si>
+  <si>
+    <t>Ability Weight</t>
+  </si>
+  <si>
+    <t>item_recipe_avalore_ring</t>
+  </si>
+  <si>
+    <t>item_avalore_ring</t>
+  </si>
+  <si>
+    <t>item_recipe_vidars_shoes</t>
+  </si>
+  <si>
+    <t>item_vidars_shoes</t>
+  </si>
+  <si>
+    <t>item_recipe_andvaranaut</t>
+  </si>
+  <si>
+    <t>item_andvaranaut</t>
+  </si>
+  <si>
+    <t>item_recipe_midas_touch</t>
+  </si>
+  <si>
+    <t>item_midas_touch</t>
+  </si>
+  <si>
+    <t>item_recipe_babr_e_bayan</t>
+  </si>
+  <si>
+    <t>item_babr_e_bayan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +373,14 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -461,7 +508,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -498,6 +545,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -509,7 +567,237 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -796,17 +1084,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA54"/>
+  <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
@@ -826,12 +1115,12 @@
     <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.42578125" customWidth="1"/>
     <col min="24" max="24" width="15.140625" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" customWidth="1"/>
-    <col min="27" max="27" width="21.7109375" customWidth="1"/>
+    <col min="25" max="26" width="14.28515625" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="8" customFormat="1">
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>73</v>
       </c>
@@ -861,202 +1150,347 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
       <c r="AA1" s="12"/>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1">
-      <c r="X3" t="e">
-        <f>INDI</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Y3" t="e">
-        <f ca="1">CONCAT(D, 14)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A4" s="9" t="s">
+      <c r="AB1" s="12"/>
+    </row>
+    <row r="2" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D2" s="9">
         <v>50</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E2" s="9">
         <v>50</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F2" s="9">
         <v>50</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G2" s="9">
         <v>10</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H2" s="9">
         <v>20</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I2" s="9">
         <v>65</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J2" s="9">
         <v>100</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K2" s="9">
         <v>10</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L2" s="9">
         <v>12</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M2" s="9">
         <v>10</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N2" s="9">
         <v>10</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O2" s="9">
         <v>35</v>
       </c>
-      <c r="S4" s="9">
+      <c r="Q2" s="9">
+        <v>5</v>
+      </c>
+      <c r="R2" s="9">
+        <v>5</v>
+      </c>
+      <c r="S2" s="9">
         <v>4</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T2" s="9">
         <v>130</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U2" s="9">
         <v>1100</v>
       </c>
-      <c r="V4" s="9">
+      <c r="V2" s="9">
         <v>250</v>
       </c>
-      <c r="W4" s="9">
+      <c r="W2" s="9">
         <v>370</v>
       </c>
-      <c r="X4" s="9">
+      <c r="X2" s="9">
         <v>3</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="Y2" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="16.5" thickTop="1">
-      <c r="A5" s="10" t="s">
+      <c r="Z2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="16.5" thickTop="1">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-    </row>
-    <row r="6" spans="1:27" ht="30">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+    </row>
+    <row r="4" spans="1:28" ht="30">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="U4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="V6" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="X4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="Z4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75">
+    <row r="5" spans="1:28" ht="15.75">
+      <c r="A5" s="2">
+        <v>3010</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75">
+      <c r="A6" s="2">
+        <v>3011</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2">
+        <f>($D$2*D6)+($E$2*E6)+($F$2*F6)+($G$2*G6)+($H$2*H6)+($I$2*I6)+($J$2*J6)+($K$2*K6)+($L$2*L6)+($M$2*M6)+($N$2*N6)+($O$2*O6)+($P$2*P6)+($Q$2*Q6)+($R$2*R6)+($S$2*S6)+($T$2*T6)+($U$2*U6)+($V$2*V6)+($W$2*W6)+($X$2*X6)+($Y$2*Y6)+($Z$2*Z6)</f>
+        <v>700</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75">
       <c r="A7" s="2">
-        <v>3010</v>
+        <v>3012</v>
       </c>
       <c r="B7" s="2">
         <v>-1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1111,19 +1545,23 @@
       <c r="Z7" s="2">
         <v>0</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="2">
+        <f t="shared" ref="AA7:AA54" si="0">($D$2*D7)+($E$2*E7)+($F$2*F7)+($G$2*G7)+($H$2*H7)+($I$2*I7)+($J$2*J7)+($K$2*K7)+($L$2*L7)+($M$2*M7)+($N$2*N7)+($O$2*O7)+($P$2*P7)+($Q$2*Q7)+($R$2*R7)+($S$2*S7)+($T$2*T7)+($U$2*U7)+($V$2*V7)+($W$2*W7)+($X$2*X7)+($Y$2*Y7)+($Z$2*Z7)</f>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75">
+    <row r="8" spans="1:28" ht="15.75">
       <c r="A8" s="2">
-        <v>3011</v>
+        <v>3013</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1135,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -1144,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1166,7 +1604,7 @@
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="2"/>
       <c r="X8" s="2">
@@ -1176,22 +1614,25 @@
         <v>0</v>
       </c>
       <c r="Z8" s="2">
-        <f>($D$4*D8)+($E$4*E8)+($F$4*F8)+($G$4*G8)+($H$4*H8)+($I$4*I8)+($J$4*J8)+($K$4*K8)+($L$4*L8)+($M$4*M8)+($N$4*N8)+($O$4*O8)+($P$4*P8)+($Q$4*Q8)+($R$4*R8)+($S$4*S8)+($T$4*T8)+($U$4*U8)+($V$4*V8)+($W$4*W8)+($X$4*X8)+($Y$4*Y8)</f>
-        <v>700</v>
-      </c>
-      <c r="AA8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+      <c r="AB8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75">
+    <row r="9" spans="1:28" ht="15.75">
       <c r="A9" s="2">
-        <v>3012</v>
+        <v>3014</v>
       </c>
       <c r="B9" s="2">
         <v>-1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -1244,22 +1685,25 @@
         <v>0</v>
       </c>
       <c r="Z9" s="2">
-        <f t="shared" ref="Z9:Z52" si="0">($D$4*D9)+($E$4*E9)+($F$4*F9)+($G$4*G9)+($H$4*H9)+($I$4*I9)+($J$4*J9)+($K$4*K9)+($L$4*L9)+($M$4*M9)+($N$4*N9)+($O$4*O9)+($P$4*P9)+($Q$4*Q9)+($R$4*R9)+($S$4*S9)+($T$4*T9)+($U$4*U9)+($V$4*V9)+($W$4*W9)+($X$4*X9)+($Y$4*Y9)</f>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75">
+    <row r="10" spans="1:28" ht="15.75">
       <c r="A10" s="2">
-        <v>3013</v>
+        <v>3015</v>
       </c>
       <c r="B10" s="2">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -1271,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -1280,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1302,7 +1746,7 @@
       </c>
       <c r="U10" s="2"/>
       <c r="V10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2">
@@ -1312,22 +1756,25 @@
         <v>0</v>
       </c>
       <c r="Z10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="2">
         <f t="shared" si="0"/>
         <v>650</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AB10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75">
+    <row r="11" spans="1:28" ht="15.75">
       <c r="A11" s="2">
-        <v>3014</v>
+        <v>3016</v>
       </c>
       <c r="B11" s="2">
         <v>-1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -1380,34 +1827,37 @@
         <v>0</v>
       </c>
       <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AB11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75">
+    <row r="12" spans="1:28" ht="15.75">
       <c r="A12" s="2">
-        <v>3015</v>
+        <v>3017</v>
       </c>
       <c r="B12" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -1416,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1448,22 +1898,25 @@
         <v>0</v>
       </c>
       <c r="Z12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="2">
         <f t="shared" si="0"/>
-        <v>650</v>
-      </c>
-      <c r="AA12" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="AB12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75">
+    <row r="13" spans="1:28" ht="15.75">
       <c r="A13" s="2">
-        <v>3016</v>
+        <v>3018</v>
       </c>
       <c r="B13" s="2">
         <v>-1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -1516,31 +1969,34 @@
         <v>0</v>
       </c>
       <c r="Z13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AB13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75">
+    <row r="14" spans="1:28" ht="15.75">
       <c r="A14" s="2">
-        <v>3017</v>
+        <v>3019</v>
       </c>
       <c r="B14" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
@@ -1552,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1584,22 +2040,25 @@
         <v>0</v>
       </c>
       <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="AA14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75">
+    <row r="15" spans="1:28" ht="15.75">
       <c r="A15" s="2">
-        <v>3018</v>
+        <v>3020</v>
       </c>
       <c r="B15" s="2">
         <v>-1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1652,28 +2111,31 @@
         <v>0</v>
       </c>
       <c r="Z15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="2" t="s">
+      <c r="AB15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75">
+    <row r="16" spans="1:28" ht="15.75">
       <c r="A16" s="2">
-        <v>3019</v>
+        <v>3021</v>
       </c>
       <c r="B16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -1688,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1720,22 +2182,25 @@
         <v>0</v>
       </c>
       <c r="Z16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="2">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="AA16" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75">
+    <row r="17" spans="1:28" ht="15.75">
       <c r="A17" s="2">
-        <v>3020</v>
+        <v>3022</v>
       </c>
       <c r="B17" s="2">
         <v>-1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -1788,22 +2253,25 @@
         <v>0</v>
       </c>
       <c r="Z17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="AB17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75">
+    <row r="18" spans="1:28" ht="15.75">
       <c r="A18" s="2">
-        <v>3021</v>
+        <v>3023</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -1824,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1856,22 +2324,25 @@
         <v>0</v>
       </c>
       <c r="Z18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="2">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="AA18" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="AB18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.75">
+    <row r="19" spans="1:28" ht="15.75">
       <c r="A19" s="2">
-        <v>3022</v>
+        <v>3024</v>
       </c>
       <c r="B19" s="2">
         <v>-1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -1924,22 +2395,25 @@
         <v>0</v>
       </c>
       <c r="Z19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="2" t="s">
+      <c r="AB19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75">
+    <row r="20" spans="1:28" ht="15.75">
       <c r="A20" s="2">
-        <v>3023</v>
+        <v>3025</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -1960,12 +2434,12 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2">
@@ -1992,22 +2466,25 @@
         <v>0</v>
       </c>
       <c r="Z20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="2">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="AA20" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="AB20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75">
+    <row r="21" spans="1:28" ht="15.75">
       <c r="A21" s="2">
-        <v>3024</v>
+        <v>3026</v>
       </c>
       <c r="B21" s="2">
         <v>-1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -2060,28 +2537,31 @@
         <v>0</v>
       </c>
       <c r="Z21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA21" s="2" t="s">
+      <c r="AB21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75">
+    <row r="22" spans="1:28" ht="15.75">
       <c r="A22" s="2">
-        <v>3025</v>
+        <v>3027</v>
       </c>
       <c r="B22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
@@ -2096,12 +2576,12 @@
         <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2">
@@ -2128,22 +2608,25 @@
         <v>0</v>
       </c>
       <c r="Z22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="2">
         <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="AA22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.75">
+    <row r="23" spans="1:28" ht="15.75">
       <c r="A23" s="2">
-        <v>3026</v>
+        <v>3028</v>
       </c>
       <c r="B23" s="2">
         <v>-1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -2196,28 +2679,31 @@
         <v>0</v>
       </c>
       <c r="Z23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA23" s="2" t="s">
+      <c r="AB23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15.75">
+    <row r="24" spans="1:28" ht="15.75">
       <c r="A24" s="2">
-        <v>3027</v>
+        <v>3029</v>
       </c>
       <c r="B24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D24" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -2264,22 +2750,25 @@
         <v>0</v>
       </c>
       <c r="Z24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="2">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="AA24" s="2" t="s">
+      <c r="AB24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15.75">
+    <row r="25" spans="1:28" ht="15.75">
       <c r="A25" s="2">
-        <v>3028</v>
+        <v>3030</v>
       </c>
       <c r="B25" s="2">
         <v>-1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -2332,25 +2821,28 @@
         <v>0</v>
       </c>
       <c r="Z25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA25" s="2" t="s">
+      <c r="AB25" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15.75">
+    <row r="26" spans="1:28" ht="15.75">
       <c r="A26" s="2">
-        <v>3029</v>
+        <v>3031</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
@@ -2368,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -2400,22 +2892,25 @@
         <v>0</v>
       </c>
       <c r="Z26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="2">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="AA26" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB26" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15.75">
+    <row r="27" spans="1:28" ht="15.75">
       <c r="A27" s="2">
-        <v>3030</v>
+        <v>3032</v>
       </c>
       <c r="B27" s="2">
         <v>-1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -2468,22 +2963,25 @@
         <v>0</v>
       </c>
       <c r="Z27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA27" s="2" t="s">
+      <c r="AB27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15.75">
+    <row r="28" spans="1:28" ht="15.75">
       <c r="A28" s="2">
-        <v>3031</v>
+        <v>3033</v>
       </c>
       <c r="B28" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -2492,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2">
         <v>0</v>
@@ -2504,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2536,22 +3034,25 @@
         <v>0</v>
       </c>
       <c r="Z28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="2">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="AA28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB28" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.75">
+    <row r="29" spans="1:28" ht="15.75">
       <c r="A29" s="2">
-        <v>3032</v>
+        <v>3034</v>
       </c>
       <c r="B29" s="2">
         <v>-1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D29" s="2">
         <v>0</v>
@@ -2604,22 +3105,25 @@
         <v>0</v>
       </c>
       <c r="Z29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA29" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="15.75">
+      <c r="AB29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="15.75">
       <c r="A30" s="2">
-        <v>3033</v>
+        <v>3035</v>
       </c>
       <c r="B30" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -2628,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
@@ -2672,22 +3176,25 @@
         <v>0</v>
       </c>
       <c r="Z30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="2">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="AA30" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" ht="15.75">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="15.75">
       <c r="A31" s="2">
-        <v>3034</v>
+        <v>3036</v>
       </c>
       <c r="B31" s="2">
         <v>-1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -2740,22 +3247,25 @@
         <v>0</v>
       </c>
       <c r="Z31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA31" s="2" t="s">
+      <c r="AB31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="15.75">
+    <row r="32" spans="1:28" ht="15.75">
       <c r="A32" s="2">
-        <v>3035</v>
+        <v>3037</v>
       </c>
       <c r="B32" s="2">
         <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
@@ -2808,22 +3318,25 @@
         <v>0</v>
       </c>
       <c r="Z32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA32" s="2" t="s">
+      <c r="AB32" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15.75">
+    <row r="33" spans="1:28" ht="15.75">
       <c r="A33" s="2">
-        <v>3036</v>
+        <v>3038</v>
       </c>
       <c r="B33" s="2">
         <v>-1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -2876,22 +3389,25 @@
         <v>0</v>
       </c>
       <c r="Z33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA33" s="2" t="s">
+      <c r="AB33" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15.75">
+    <row r="34" spans="1:28" ht="15.75">
       <c r="A34" s="2">
-        <v>3037</v>
+        <v>3039</v>
       </c>
       <c r="B34" s="2">
         <v>30</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
@@ -2944,22 +3460,25 @@
         <v>0</v>
       </c>
       <c r="Z34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA34" s="2" t="s">
+      <c r="AB34" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="15.75">
+    <row r="35" spans="1:28" ht="15.75">
       <c r="A35" s="2">
-        <v>3038</v>
+        <v>3040</v>
       </c>
       <c r="B35" s="2">
         <v>-1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3012,22 +3531,25 @@
         <v>0</v>
       </c>
       <c r="Z35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA35" s="2" t="s">
+      <c r="AB35" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15.75">
+    <row r="36" spans="1:28" ht="15.75">
       <c r="A36" s="2">
-        <v>3039</v>
+        <v>3041</v>
       </c>
       <c r="B36" s="2">
         <v>30</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D36" s="2">
         <v>0</v>
@@ -3080,22 +3602,25 @@
         <v>0</v>
       </c>
       <c r="Z36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA36" s="2" t="s">
+      <c r="AB36" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="15.75">
+    <row r="37" spans="1:28" ht="15.75">
       <c r="A37" s="2">
-        <v>3040</v>
+        <v>3042</v>
       </c>
       <c r="B37" s="2">
         <v>-1</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3148,22 +3673,25 @@
         <v>0</v>
       </c>
       <c r="Z37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA37" s="2" t="s">
+      <c r="AB37" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="15.75">
+    <row r="38" spans="1:28" ht="15.75">
       <c r="A38" s="2">
-        <v>3041</v>
+        <v>3043</v>
       </c>
       <c r="B38" s="2">
         <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3216,22 +3744,25 @@
         <v>0</v>
       </c>
       <c r="Z38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA38" s="2" t="s">
+      <c r="AB38" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.75">
+    <row r="39" spans="1:28" ht="15.75">
       <c r="A39" s="2">
-        <v>3042</v>
+        <v>3044</v>
       </c>
       <c r="B39" s="2">
         <v>-1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D39" s="2">
         <v>0</v>
@@ -3284,22 +3815,25 @@
         <v>0</v>
       </c>
       <c r="Z39" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA39" s="2" t="s">
+      <c r="AB39" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15.75">
+    <row r="40" spans="1:28" ht="15.75">
       <c r="A40" s="2">
-        <v>3043</v>
+        <v>3045</v>
       </c>
       <c r="B40" s="2">
         <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D40" s="2">
         <v>0</v>
@@ -3342,7 +3876,7 @@
       </c>
       <c r="U40" s="2"/>
       <c r="V40" s="2">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="W40" s="2"/>
       <c r="X40" s="2">
@@ -3352,22 +3886,25 @@
         <v>0</v>
       </c>
       <c r="Z40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA40" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB40" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15.75">
+    <row r="41" spans="1:28" ht="15.75">
       <c r="A41" s="2">
-        <v>3044</v>
+        <v>3046</v>
       </c>
       <c r="B41" s="2">
         <v>-1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D41" s="2">
         <v>0</v>
@@ -3420,22 +3957,25 @@
         <v>0</v>
       </c>
       <c r="Z41" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA41" s="2" t="s">
+      <c r="AB41" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="15.75">
+    <row r="42" spans="1:28" ht="15.75">
       <c r="A42" s="2">
-        <v>3045</v>
+        <v>3047</v>
       </c>
       <c r="B42" s="2">
         <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D42" s="2">
         <v>0</v>
@@ -3474,11 +4014,11 @@
         <v>0</v>
       </c>
       <c r="T42" s="2">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="U42" s="2"/>
       <c r="V42" s="2">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="W42" s="2"/>
       <c r="X42" s="2">
@@ -3488,22 +4028,25 @@
         <v>0</v>
       </c>
       <c r="Z42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="2">
         <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-      <c r="AA42" s="2" t="s">
+        <v>162.5</v>
+      </c>
+      <c r="AB42" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="30">
+    <row r="43" spans="1:28" ht="15.75">
       <c r="A43" s="2">
-        <v>3046</v>
+        <v>3048</v>
       </c>
       <c r="B43" s="2">
         <v>-1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D43" s="2">
         <v>0</v>
@@ -3556,22 +4099,25 @@
         <v>0</v>
       </c>
       <c r="Z43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA43" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" ht="15.75">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="2">
+        <f>($D$2*D43)+($E$2*E43)+($F$2*F43)+($G$2*G43)+($H$2*H43)+($I$2*I43)+($J$2*J43)+($K$2*K43)+($L$2*L43)+($M$2*M43)+($N$2*N43)+($O$2*O43)+($P$2*P43)+($Q$2*Q43)+($R$2*R43)+($S$2*S43)+($T$2*T43)+($U$2*U43)+($V$2*V43)+($W$2*W43)+($X$2*X43)+($Y$2*Y43)+($Z$2*Z43)</f>
+        <v>0</v>
+      </c>
+      <c r="AB43" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="15.75">
       <c r="A44" s="2">
-        <v>3047</v>
+        <v>3049</v>
       </c>
       <c r="B44" s="2">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D44" s="2">
         <v>0</v>
@@ -3583,7 +4129,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H44" s="2">
         <v>0</v>
@@ -3610,11 +4156,11 @@
         <v>0</v>
       </c>
       <c r="T44" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="U44" s="2"/>
       <c r="V44" s="2">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="W44" s="2"/>
       <c r="X44" s="2">
@@ -3624,22 +4170,25 @@
         <v>0</v>
       </c>
       <c r="Z44" s="2">
-        <f>($D$4*D44)+($E$4*E44)+($F$4*F44)+($G$4*G44)+($H$4*H44)+($I$4*I44)+($J$4*J44)+($K$4*K44)+($L$4*L44)+($M$4*M44)+($N$4*N44)+($O$4*O44)+($P$4*P44)+($Q$4*Q44)+($R$4*R44)+($S$4*S44)+($T$4*T44)+($U$4*U44)+($V$4*V44)+($W$4*W44)+($X$4*X44)+($Y$4*Y44)</f>
-        <v>162.5</v>
-      </c>
-      <c r="AA44" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" ht="15.75">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="2">
+        <f t="shared" si="0"/>
+        <v>712.5</v>
+      </c>
+      <c r="AB44" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="15.75">
       <c r="A45" s="2">
-        <v>3048</v>
+        <v>3050</v>
       </c>
       <c r="B45" s="2">
         <v>-1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D45" s="2">
         <v>0</v>
@@ -3692,22 +4241,25 @@
         <v>0</v>
       </c>
       <c r="Z45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA45" s="2" t="s">
+      <c r="AB45" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="15.75">
+    <row r="46" spans="1:28" ht="15.75">
       <c r="A46" s="2">
-        <v>3049</v>
+        <v>3051</v>
       </c>
       <c r="B46" s="2">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
@@ -3719,7 +4271,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
@@ -3728,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -3750,7 +4302,7 @@
       </c>
       <c r="U46" s="2"/>
       <c r="V46" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="W46" s="2"/>
       <c r="X46" s="2">
@@ -3760,22 +4312,25 @@
         <v>0</v>
       </c>
       <c r="Z46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="2">
         <f t="shared" si="0"/>
-        <v>712.5</v>
-      </c>
-      <c r="AA46" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="AB46" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="15.75">
+    <row r="47" spans="1:28" ht="15.75">
       <c r="A47" s="2">
-        <v>3050</v>
+        <v>3052</v>
       </c>
       <c r="B47" s="2">
         <v>-1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D47" s="2">
         <v>0</v>
@@ -3828,22 +4383,25 @@
         <v>0</v>
       </c>
       <c r="Z47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA47" s="2" t="s">
+      <c r="AB47" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15.75">
+    <row r="48" spans="1:28" ht="15.75">
       <c r="A48" s="2">
-        <v>3051</v>
+        <v>3053</v>
       </c>
       <c r="B48" s="2">
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D48" s="2">
         <v>0</v>
@@ -3855,16 +4413,16 @@
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="H48" s="2">
         <v>0</v>
       </c>
       <c r="I48" s="2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -3896,22 +4454,25 @@
         <v>0</v>
       </c>
       <c r="Z48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="2">
         <f t="shared" si="0"/>
-        <v>1100</v>
-      </c>
-      <c r="AA48" s="2" t="s">
+        <v>3575</v>
+      </c>
+      <c r="AB48" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="15.75">
+    <row r="49" spans="1:28" ht="15.75">
       <c r="A49" s="2">
-        <v>3052</v>
+        <v>3054</v>
       </c>
       <c r="B49" s="2">
         <v>-1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D49" s="2">
         <v>0</v>
@@ -3964,22 +4525,25 @@
         <v>0</v>
       </c>
       <c r="Z49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA49" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27" ht="15.75">
+      <c r="AB49" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="15.75">
       <c r="A50" s="2">
-        <v>3053</v>
+        <v>3055</v>
       </c>
       <c r="B50" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D50" s="2">
         <v>0</v>
@@ -3991,13 +4555,13 @@
         <v>0</v>
       </c>
       <c r="G50" s="2">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="H50" s="2">
         <v>0</v>
       </c>
       <c r="I50" s="2">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="J50" s="2">
         <v>0</v>
@@ -4032,158 +4596,199 @@
         <v>0</v>
       </c>
       <c r="Z50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="2">
         <f t="shared" si="0"/>
-        <v>3575</v>
-      </c>
-      <c r="AA50" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27" ht="15.75">
-      <c r="A51" s="2">
-        <v>3054</v>
-      </c>
-      <c r="B51" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="15.75">
+      <c r="A51" s="13">
+        <v>3056</v>
+      </c>
+      <c r="B51" s="13">
         <v>-1</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2">
-        <v>0</v>
-      </c>
-      <c r="F51" s="2">
-        <v>0</v>
-      </c>
-      <c r="G51" s="2">
-        <v>0</v>
-      </c>
-      <c r="H51" s="2">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <v>0</v>
-      </c>
-      <c r="J51" s="2">
-        <v>0</v>
-      </c>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2">
-        <v>0</v>
-      </c>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2">
-        <v>0</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="2">
-        <v>0</v>
-      </c>
-      <c r="T51" s="2">
-        <v>0</v>
-      </c>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2">
-        <v>0</v>
-      </c>
-      <c r="W51" s="2"/>
-      <c r="X51" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="2">
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="13">
+        <v>0</v>
+      </c>
+      <c r="E51" s="13">
+        <v>0</v>
+      </c>
+      <c r="F51" s="13">
+        <v>0</v>
+      </c>
+      <c r="G51" s="13">
+        <v>0</v>
+      </c>
+      <c r="H51" s="13">
+        <v>0</v>
+      </c>
+      <c r="I51" s="13">
+        <v>0</v>
+      </c>
+      <c r="J51" s="13">
+        <v>0</v>
+      </c>
+      <c r="K51" s="13">
+        <v>0</v>
+      </c>
+      <c r="L51" s="13">
+        <v>0</v>
+      </c>
+      <c r="M51" s="13">
+        <v>0</v>
+      </c>
+      <c r="N51" s="13">
+        <v>0</v>
+      </c>
+      <c r="O51" s="13">
+        <v>0</v>
+      </c>
+      <c r="P51" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="13">
+        <v>0</v>
+      </c>
+      <c r="R51" s="13">
+        <v>0</v>
+      </c>
+      <c r="S51" s="13">
+        <v>0</v>
+      </c>
+      <c r="T51" s="13">
+        <v>0</v>
+      </c>
+      <c r="U51" s="13">
+        <v>0</v>
+      </c>
+      <c r="V51" s="13">
+        <v>0</v>
+      </c>
+      <c r="W51" s="13">
+        <v>0</v>
+      </c>
+      <c r="X51" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="13">
         <v>0</v>
       </c>
       <c r="Z51" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA51" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27" ht="15.75">
-      <c r="A52" s="2">
-        <v>3055</v>
-      </c>
-      <c r="B52" s="2">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0</v>
-      </c>
-      <c r="F52" s="2">
-        <v>0</v>
-      </c>
-      <c r="G52" s="2">
-        <v>0</v>
-      </c>
-      <c r="H52" s="2">
-        <v>0</v>
-      </c>
-      <c r="I52" s="2">
-        <v>0</v>
-      </c>
-      <c r="J52" s="2">
-        <v>0</v>
-      </c>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2">
-        <v>0</v>
-      </c>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2">
-        <v>0</v>
-      </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="2">
-        <v>0</v>
-      </c>
-      <c r="T52" s="2">
-        <v>0</v>
-      </c>
-      <c r="U52" s="2"/>
-      <c r="V52" s="2">
-        <v>0</v>
-      </c>
-      <c r="W52" s="2"/>
-      <c r="X52" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="2">
+      <c r="AB51" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="15.75">
+      <c r="A52" s="13">
+        <v>3057</v>
+      </c>
+      <c r="B52" s="13">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="13">
+        <v>0</v>
+      </c>
+      <c r="E52" s="13">
+        <v>0</v>
+      </c>
+      <c r="F52" s="13">
+        <v>0</v>
+      </c>
+      <c r="G52" s="13">
+        <v>0</v>
+      </c>
+      <c r="H52" s="13">
+        <v>0</v>
+      </c>
+      <c r="I52" s="13">
+        <v>0</v>
+      </c>
+      <c r="J52" s="13">
+        <v>4</v>
+      </c>
+      <c r="K52" s="13">
+        <v>0</v>
+      </c>
+      <c r="L52" s="13">
+        <v>0</v>
+      </c>
+      <c r="M52" s="13">
+        <v>0</v>
+      </c>
+      <c r="N52" s="13">
+        <v>0</v>
+      </c>
+      <c r="O52" s="13">
+        <v>0</v>
+      </c>
+      <c r="P52" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="13">
+        <v>0</v>
+      </c>
+      <c r="R52" s="13">
+        <v>0</v>
+      </c>
+      <c r="S52" s="13">
+        <v>0</v>
+      </c>
+      <c r="T52" s="13">
+        <v>0</v>
+      </c>
+      <c r="U52" s="13">
+        <v>0</v>
+      </c>
+      <c r="V52" s="13">
+        <v>0</v>
+      </c>
+      <c r="W52" s="13">
+        <v>0</v>
+      </c>
+      <c r="X52" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="13">
         <v>0</v>
       </c>
       <c r="Z52" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA52" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27" ht="15.75">
+        <v>400</v>
+      </c>
+      <c r="AB52" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" ht="15.75">
       <c r="A53" s="13">
-        <v>3056</v>
+        <v>3058</v>
       </c>
       <c r="B53" s="13">
         <v>-1</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D53" s="13">
         <v>0</v>
@@ -4251,28 +4856,1005 @@
       <c r="Y53" s="13">
         <v>0</v>
       </c>
-      <c r="AA53" s="13" t="s">
+      <c r="Z53" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB53" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" ht="15.75">
+      <c r="A54" s="13">
+        <v>3059</v>
+      </c>
+      <c r="B54" s="13">
+        <v>30</v>
+      </c>
+      <c r="C54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="13">
+        <v>0</v>
+      </c>
+      <c r="E54" s="13">
+        <v>0</v>
+      </c>
+      <c r="F54" s="13">
+        <v>0</v>
+      </c>
+      <c r="G54" s="13">
+        <v>0</v>
+      </c>
+      <c r="H54" s="13">
+        <v>0</v>
+      </c>
+      <c r="I54" s="13">
+        <v>0</v>
+      </c>
+      <c r="J54" s="13">
+        <v>0</v>
+      </c>
+      <c r="K54" s="13">
+        <v>0</v>
+      </c>
+      <c r="L54" s="13">
+        <v>0</v>
+      </c>
+      <c r="M54" s="13">
+        <v>0</v>
+      </c>
+      <c r="N54" s="13">
+        <v>0</v>
+      </c>
+      <c r="O54" s="13">
+        <v>0</v>
+      </c>
+      <c r="P54" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="13">
+        <v>0</v>
+      </c>
+      <c r="R54" s="13">
+        <v>0</v>
+      </c>
+      <c r="S54" s="13">
+        <v>0</v>
+      </c>
+      <c r="T54" s="13">
+        <v>0</v>
+      </c>
+      <c r="U54" s="13">
+        <v>0</v>
+      </c>
+      <c r="V54" s="13">
+        <v>0</v>
+      </c>
+      <c r="W54" s="13">
+        <v>0</v>
+      </c>
+      <c r="X54" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>440</v>
+      </c>
+      <c r="AA54" s="2">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="AB54" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" ht="15.75">
+      <c r="A55" s="13">
+        <v>3060</v>
+      </c>
+      <c r="B55" s="13">
+        <v>-1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="13">
+        <v>0</v>
+      </c>
+      <c r="E55" s="13">
+        <v>0</v>
+      </c>
+      <c r="F55" s="13">
+        <v>0</v>
+      </c>
+      <c r="G55" s="13">
+        <v>0</v>
+      </c>
+      <c r="H55" s="13">
+        <v>0</v>
+      </c>
+      <c r="I55" s="13">
+        <v>0</v>
+      </c>
+      <c r="J55" s="13">
+        <v>0</v>
+      </c>
+      <c r="K55" s="13">
+        <v>0</v>
+      </c>
+      <c r="L55" s="13">
+        <v>0</v>
+      </c>
+      <c r="M55" s="13">
+        <v>0</v>
+      </c>
+      <c r="N55" s="13">
+        <v>0</v>
+      </c>
+      <c r="O55" s="13">
+        <v>0</v>
+      </c>
+      <c r="P55" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="13">
+        <v>0</v>
+      </c>
+      <c r="R55" s="13">
+        <v>0</v>
+      </c>
+      <c r="S55" s="13">
+        <v>0</v>
+      </c>
+      <c r="T55" s="13">
+        <v>0</v>
+      </c>
+      <c r="U55" s="13">
+        <v>0</v>
+      </c>
+      <c r="V55" s="13">
+        <v>0</v>
+      </c>
+      <c r="W55" s="13">
+        <v>0</v>
+      </c>
+      <c r="X55" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="2">
+        <f t="shared" ref="AA7:AA70" si="1">($D$2*D55)+($E$2*E55)+($F$2*F55)+($G$2*G55)+($H$2*H55)+($I$2*I55)+($J$2*J55)+($K$2*K55)+($L$2*L55)+($M$2*M55)+($N$2*N55)+($O$2*O55)+($P$2*P55)+($Q$2*Q55)+($R$2*R55)+($S$2*S55)+($T$2*T55)+($U$2*U55)+($V$2*V55)+($W$2*W55)+($X$2*X55)+($Y$2*Y55)</f>
+        <v>0</v>
+      </c>
+      <c r="AB55" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="15.75">
-      <c r="A54" s="13">
-        <v>3057</v>
-      </c>
-      <c r="B54" s="13">
+    <row r="56" spans="1:28" ht="15.75">
+      <c r="A56" s="13">
+        <v>3061</v>
+      </c>
+      <c r="B56" s="13">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="13">
+        <v>0</v>
+      </c>
+      <c r="E56" s="13">
+        <v>0</v>
+      </c>
+      <c r="F56" s="13">
+        <v>0</v>
+      </c>
+      <c r="G56" s="13">
+        <v>0</v>
+      </c>
+      <c r="H56" s="13">
+        <v>0</v>
+      </c>
+      <c r="I56" s="13">
+        <v>0</v>
+      </c>
+      <c r="J56" s="13">
+        <v>2</v>
+      </c>
+      <c r="K56" s="13">
+        <v>0</v>
+      </c>
+      <c r="L56" s="13">
+        <v>0</v>
+      </c>
+      <c r="M56" s="13">
+        <v>0</v>
+      </c>
+      <c r="N56" s="13">
+        <v>0</v>
+      </c>
+      <c r="O56" s="13">
+        <v>0</v>
+      </c>
+      <c r="P56" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="13">
+        <v>0</v>
+      </c>
+      <c r="R56" s="13">
+        <v>0</v>
+      </c>
+      <c r="S56" s="13">
+        <v>0</v>
+      </c>
+      <c r="T56" s="13">
+        <v>0</v>
+      </c>
+      <c r="U56" s="13">
+        <v>0</v>
+      </c>
+      <c r="V56" s="13">
+        <v>0</v>
+      </c>
+      <c r="W56" s="13">
+        <v>0</v>
+      </c>
+      <c r="X56" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="AB56" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="15.75">
+      <c r="A57" s="13">
+        <v>3062</v>
+      </c>
+      <c r="B57" s="13">
+        <v>-1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="13">
+        <v>0</v>
+      </c>
+      <c r="E57" s="13">
+        <v>0</v>
+      </c>
+      <c r="F57" s="13">
+        <v>0</v>
+      </c>
+      <c r="G57" s="13">
+        <v>0</v>
+      </c>
+      <c r="H57" s="13">
+        <v>0</v>
+      </c>
+      <c r="I57" s="13">
+        <v>0</v>
+      </c>
+      <c r="J57" s="13">
+        <v>0</v>
+      </c>
+      <c r="K57" s="13">
+        <v>0</v>
+      </c>
+      <c r="L57" s="13">
+        <v>0</v>
+      </c>
+      <c r="M57" s="13">
+        <v>0</v>
+      </c>
+      <c r="N57" s="13">
+        <v>0</v>
+      </c>
+      <c r="O57" s="13">
+        <v>0</v>
+      </c>
+      <c r="P57" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="13">
+        <v>0</v>
+      </c>
+      <c r="R57" s="13">
+        <v>0</v>
+      </c>
+      <c r="S57" s="13">
+        <v>0</v>
+      </c>
+      <c r="T57" s="13">
+        <v>0</v>
+      </c>
+      <c r="U57" s="13">
+        <v>0</v>
+      </c>
+      <c r="V57" s="13">
+        <v>0</v>
+      </c>
+      <c r="W57" s="13">
+        <v>0</v>
+      </c>
+      <c r="X57" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" s="16" customFormat="1" ht="15.75">
+      <c r="A58" s="15">
+        <v>3063</v>
+      </c>
+      <c r="B58" s="15">
+        <v>4</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="15">
+        <v>0</v>
+      </c>
+      <c r="E58" s="15">
+        <v>0</v>
+      </c>
+      <c r="F58" s="15">
+        <v>0</v>
+      </c>
+      <c r="G58" s="15">
+        <v>0</v>
+      </c>
+      <c r="H58" s="15">
+        <v>0</v>
+      </c>
+      <c r="I58" s="15">
+        <v>0</v>
+      </c>
+      <c r="J58" s="15">
+        <v>0</v>
+      </c>
+      <c r="K58" s="15">
+        <v>0</v>
+      </c>
+      <c r="L58" s="15">
+        <v>0</v>
+      </c>
+      <c r="M58" s="15">
+        <v>0</v>
+      </c>
+      <c r="N58" s="15">
+        <v>0</v>
+      </c>
+      <c r="O58" s="15">
+        <v>0</v>
+      </c>
+      <c r="P58" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="15">
+        <v>0</v>
+      </c>
+      <c r="R58" s="15">
+        <v>0</v>
+      </c>
+      <c r="S58" s="15">
+        <v>0</v>
+      </c>
+      <c r="T58" s="15">
+        <v>0</v>
+      </c>
+      <c r="U58" s="15">
+        <v>0</v>
+      </c>
+      <c r="V58" s="15">
+        <v>0</v>
+      </c>
+      <c r="W58" s="15">
+        <v>0</v>
+      </c>
+      <c r="X58" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y58" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA58" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" ht="15.75">
+      <c r="A59" s="13">
+        <v>3064</v>
+      </c>
+      <c r="B59" s="13">
+        <v>-1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="13">
+        <v>0</v>
+      </c>
+      <c r="E59" s="13">
+        <v>0</v>
+      </c>
+      <c r="F59" s="13">
+        <v>0</v>
+      </c>
+      <c r="G59" s="13">
+        <v>0</v>
+      </c>
+      <c r="H59" s="13">
+        <v>0</v>
+      </c>
+      <c r="I59" s="13">
+        <v>0</v>
+      </c>
+      <c r="J59" s="13">
+        <v>0</v>
+      </c>
+      <c r="K59" s="13">
+        <v>0</v>
+      </c>
+      <c r="L59" s="13">
+        <v>0</v>
+      </c>
+      <c r="M59" s="13">
+        <v>0</v>
+      </c>
+      <c r="N59" s="13">
+        <v>0</v>
+      </c>
+      <c r="O59" s="13">
+        <v>0</v>
+      </c>
+      <c r="P59" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="13">
+        <v>0</v>
+      </c>
+      <c r="R59" s="13">
+        <v>0</v>
+      </c>
+      <c r="S59" s="13">
+        <v>0</v>
+      </c>
+      <c r="T59" s="13">
+        <v>0</v>
+      </c>
+      <c r="U59" s="13">
+        <v>0</v>
+      </c>
+      <c r="V59" s="13">
+        <v>0</v>
+      </c>
+      <c r="W59" s="13">
+        <v>0</v>
+      </c>
+      <c r="X59" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA59" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" ht="15.75">
+      <c r="A60" s="13">
+        <v>3065</v>
+      </c>
+      <c r="B60" s="13">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="13">
+        <v>0</v>
+      </c>
+      <c r="E60" s="13">
+        <v>0</v>
+      </c>
+      <c r="F60" s="13">
+        <v>0</v>
+      </c>
+      <c r="G60" s="13">
+        <v>0</v>
+      </c>
+      <c r="H60" s="13">
+        <v>0</v>
+      </c>
+      <c r="I60" s="13">
+        <v>0</v>
+      </c>
+      <c r="J60" s="13">
+        <v>2</v>
+      </c>
+      <c r="K60" s="13">
+        <v>0</v>
+      </c>
+      <c r="L60" s="13">
+        <v>0</v>
+      </c>
+      <c r="M60" s="13">
+        <v>0</v>
+      </c>
+      <c r="N60" s="13">
+        <v>0</v>
+      </c>
+      <c r="O60" s="13">
+        <v>0</v>
+      </c>
+      <c r="P60" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="13">
+        <v>0</v>
+      </c>
+      <c r="R60" s="13">
+        <v>0</v>
+      </c>
+      <c r="S60" s="13">
+        <v>0</v>
+      </c>
+      <c r="T60" s="13">
+        <v>0</v>
+      </c>
+      <c r="U60" s="13">
+        <v>0</v>
+      </c>
+      <c r="V60" s="13">
+        <v>0</v>
+      </c>
+      <c r="W60" s="13">
+        <v>0</v>
+      </c>
+      <c r="X60" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="13">
+        <v>440</v>
+      </c>
+      <c r="AA60" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" ht="15.75">
+      <c r="A61" s="13">
+        <v>3066</v>
+      </c>
+      <c r="B61" s="13">
+        <v>-1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0</v>
+      </c>
+      <c r="E61" s="13">
+        <v>0</v>
+      </c>
+      <c r="F61" s="13">
+        <v>0</v>
+      </c>
+      <c r="G61" s="13">
+        <v>0</v>
+      </c>
+      <c r="H61" s="13">
+        <v>0</v>
+      </c>
+      <c r="I61" s="13">
+        <v>0</v>
+      </c>
+      <c r="J61" s="13">
+        <v>0</v>
+      </c>
+      <c r="K61" s="13">
+        <v>0</v>
+      </c>
+      <c r="L61" s="13">
+        <v>0</v>
+      </c>
+      <c r="M61" s="13">
+        <v>0</v>
+      </c>
+      <c r="N61" s="13">
+        <v>0</v>
+      </c>
+      <c r="O61" s="13">
+        <v>0</v>
+      </c>
+      <c r="P61" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="13">
+        <v>0</v>
+      </c>
+      <c r="R61" s="13">
+        <v>0</v>
+      </c>
+      <c r="S61" s="13">
+        <v>0</v>
+      </c>
+      <c r="T61" s="13">
+        <v>0</v>
+      </c>
+      <c r="U61" s="13">
+        <v>0</v>
+      </c>
+      <c r="V61" s="13">
+        <v>0</v>
+      </c>
+      <c r="W61" s="13">
+        <v>0</v>
+      </c>
+      <c r="X61" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA61" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" ht="15.75">
+      <c r="A62" s="13">
+        <v>3067</v>
+      </c>
+      <c r="B62" s="13">
         <v>3</v>
       </c>
-      <c r="C54" t="s">
-        <v>81</v>
+      <c r="C62" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="13">
+        <v>0</v>
+      </c>
+      <c r="E62" s="13">
+        <v>0</v>
+      </c>
+      <c r="F62" s="13">
+        <v>0</v>
+      </c>
+      <c r="G62" s="13">
+        <v>0</v>
+      </c>
+      <c r="H62" s="13">
+        <v>0</v>
+      </c>
+      <c r="I62" s="13">
+        <v>0</v>
+      </c>
+      <c r="J62" s="13">
+        <v>0</v>
+      </c>
+      <c r="K62" s="13">
+        <v>0</v>
+      </c>
+      <c r="L62" s="13">
+        <v>0</v>
+      </c>
+      <c r="M62" s="13">
+        <v>0</v>
+      </c>
+      <c r="N62" s="13">
+        <v>0</v>
+      </c>
+      <c r="O62" s="13">
+        <v>0</v>
+      </c>
+      <c r="P62" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="13">
+        <v>0</v>
+      </c>
+      <c r="R62" s="13">
+        <v>0</v>
+      </c>
+      <c r="S62" s="13">
+        <v>0</v>
+      </c>
+      <c r="T62" s="13">
+        <v>0</v>
+      </c>
+      <c r="U62" s="13">
+        <v>0</v>
+      </c>
+      <c r="V62" s="13">
+        <v>0</v>
+      </c>
+      <c r="W62" s="13">
+        <v>0</v>
+      </c>
+      <c r="X62" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" ht="15.75">
+      <c r="A63" s="13">
+        <v>3068</v>
+      </c>
+      <c r="B63" s="13">
+        <v>-1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="13">
+        <v>0</v>
+      </c>
+      <c r="E63" s="13">
+        <v>0</v>
+      </c>
+      <c r="F63" s="13">
+        <v>0</v>
+      </c>
+      <c r="G63" s="13">
+        <v>0</v>
+      </c>
+      <c r="H63" s="13">
+        <v>0</v>
+      </c>
+      <c r="I63" s="13">
+        <v>0</v>
+      </c>
+      <c r="J63" s="13">
+        <v>0</v>
+      </c>
+      <c r="K63" s="13">
+        <v>0</v>
+      </c>
+      <c r="L63" s="13">
+        <v>0</v>
+      </c>
+      <c r="M63" s="13">
+        <v>0</v>
+      </c>
+      <c r="N63" s="13">
+        <v>0</v>
+      </c>
+      <c r="O63" s="13">
+        <v>0</v>
+      </c>
+      <c r="P63" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="13">
+        <v>0</v>
+      </c>
+      <c r="R63" s="13">
+        <v>0</v>
+      </c>
+      <c r="S63" s="13">
+        <v>0</v>
+      </c>
+      <c r="T63" s="13">
+        <v>0</v>
+      </c>
+      <c r="U63" s="13">
+        <v>0</v>
+      </c>
+      <c r="V63" s="13">
+        <v>0</v>
+      </c>
+      <c r="W63" s="13">
+        <v>0</v>
+      </c>
+      <c r="X63" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA63" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" ht="15.75">
+      <c r="A64" s="13">
+        <v>3069</v>
+      </c>
+      <c r="B64" s="13">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>94</v>
+      </c>
+      <c r="D64" s="13">
+        <v>0</v>
+      </c>
+      <c r="E64" s="13">
+        <v>0</v>
+      </c>
+      <c r="F64" s="13">
+        <v>0</v>
+      </c>
+      <c r="G64" s="13">
+        <v>0</v>
+      </c>
+      <c r="H64" s="13">
+        <v>0</v>
+      </c>
+      <c r="I64" s="13">
+        <v>0</v>
+      </c>
+      <c r="J64" s="13">
+        <v>6</v>
+      </c>
+      <c r="K64" s="13">
+        <v>0</v>
+      </c>
+      <c r="L64" s="13">
+        <v>0</v>
+      </c>
+      <c r="M64" s="13">
+        <v>0</v>
+      </c>
+      <c r="N64" s="13">
+        <v>0</v>
+      </c>
+      <c r="O64" s="13">
+        <v>0</v>
+      </c>
+      <c r="P64" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="13">
+        <v>50</v>
+      </c>
+      <c r="R64" s="13">
+        <v>50</v>
+      </c>
+      <c r="S64" s="13">
+        <v>0</v>
+      </c>
+      <c r="T64" s="13">
+        <v>0</v>
+      </c>
+      <c r="U64" s="13">
+        <v>0</v>
+      </c>
+      <c r="V64" s="13">
+        <v>0</v>
+      </c>
+      <c r="W64" s="13">
+        <v>0</v>
+      </c>
+      <c r="X64" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="2">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="65" spans="27:27" ht="15.75">
+      <c r="AA65" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="27:27" ht="15.75">
+      <c r="AA66" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="27:27" ht="15.75">
+      <c r="AA67" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="27:27" ht="15.75">
+      <c r="AA68" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="27:27" ht="15.75">
+      <c r="AA69" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="27:27" ht="15.75">
+      <c r="AA70" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="27:27" ht="15.75">
+      <c r="AA71" s="2">
+        <f t="shared" ref="AA71:AA72" si="2">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="27:27" ht="15.75">
+      <c r="AA72" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A5:AA5"/>
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A3:AB3"/>
+    <mergeCell ref="A1:AB1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:AA1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A3:AB1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
item tree + golden fleece
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>item_solar_crown</t>
+  </si>
+  <si>
+    <t>item_recipe_golden_fleece</t>
+  </si>
+  <si>
+    <t>item_golden_fleece</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -512,6 +518,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -524,7 +539,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -575,6 +590,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -587,7 +608,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -876,9 +927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="M66" sqref="M66"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1590" topLeftCell="A40" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1344,7 +1395,7 @@
       </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2">
-        <f t="shared" ref="AB7:AB67" si="0">($D$2*D7)+($E$2*E7)+($F$2*F7)+($G$2*G7)+($H$2*H7)+($I$2*I7)+($J$2*J7)+($K$2*K7)+($L$2*L7)+($M$2*M7)+($N$2*N7)+($O$2*O7)+($P$2*P7)+($Q$2*Q7)+($R$2*R7)+($S$2*S7)+($T$2*T7)+($U$2*U7)+($V$2*V7)+($W$2*W7)+($X$2*X7)+($Y$2*Y7)+($Z$2*Z7)+(AA7)</f>
+        <f t="shared" ref="AB7:AB68" si="0">($D$2*D7)+($E$2*E7)+($F$2*F7)+($G$2*G7)+($H$2*H7)+($I$2*I7)+($J$2*J7)+($K$2*K7)+($L$2*L7)+($M$2*M7)+($N$2*N7)+($O$2*O7)+($P$2*P7)+($Q$2*Q7)+($R$2*R7)+($S$2*S7)+($T$2*T7)+($U$2*U7)+($V$2*V7)+($W$2*W7)+($X$2*X7)+($Y$2*Y7)+($Z$2*Z7)+(AA7)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="2" t="s">
@@ -3284,12 +3335,12 @@
         <v>0</v>
       </c>
       <c r="Z34" s="2">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AC34" s="2" t="s">
         <v>40</v>
@@ -5701,6 +5752,42 @@
       <c r="N65" s="8">
         <v>0</v>
       </c>
+      <c r="O65" s="8">
+        <v>0</v>
+      </c>
+      <c r="P65" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="8">
+        <v>0</v>
+      </c>
+      <c r="R65" s="8">
+        <v>0</v>
+      </c>
+      <c r="S65" s="8">
+        <v>0</v>
+      </c>
+      <c r="T65" s="8">
+        <v>0</v>
+      </c>
+      <c r="U65" s="8">
+        <v>0</v>
+      </c>
+      <c r="V65" s="8">
+        <v>0</v>
+      </c>
+      <c r="W65" s="8">
+        <v>0</v>
+      </c>
+      <c r="X65" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="8">
+        <v>0</v>
+      </c>
       <c r="AB65" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5746,21 +5833,223 @@
       <c r="M66" s="8">
         <v>0</v>
       </c>
+      <c r="N66" s="8">
+        <v>0</v>
+      </c>
+      <c r="O66" s="20">
+        <v>0</v>
+      </c>
+      <c r="P66" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="21">
+        <v>0</v>
+      </c>
+      <c r="R66" s="21">
+        <v>0</v>
+      </c>
+      <c r="S66" s="21">
+        <v>0</v>
+      </c>
+      <c r="T66" s="21">
+        <v>0</v>
+      </c>
+      <c r="U66" s="21">
+        <v>0</v>
+      </c>
+      <c r="V66" s="21">
+        <v>0</v>
+      </c>
+      <c r="W66" s="21">
+        <v>0</v>
+      </c>
+      <c r="X66" s="21">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA66">
+        <f>AB16+AB34+AB68</f>
+        <v>1375</v>
+      </c>
       <c r="AB66" s="2">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="15.75">
+      <c r="A67" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C67" s="8">
+        <v>3072</v>
+      </c>
+      <c r="D67" s="8">
+        <v>0</v>
+      </c>
+      <c r="E67" s="8">
+        <v>0</v>
+      </c>
+      <c r="F67" s="8">
+        <v>0</v>
+      </c>
+      <c r="G67" s="8">
+        <v>0</v>
+      </c>
+      <c r="H67" s="8">
+        <v>0</v>
+      </c>
+      <c r="I67" s="8">
+        <v>0</v>
+      </c>
+      <c r="J67" s="8">
+        <v>0</v>
+      </c>
+      <c r="K67" s="8">
+        <v>0</v>
+      </c>
+      <c r="L67" s="8">
+        <v>0</v>
+      </c>
+      <c r="M67" s="8">
+        <v>0</v>
+      </c>
+      <c r="N67" s="20">
+        <v>0</v>
+      </c>
+      <c r="O67" s="21">
+        <v>0</v>
+      </c>
+      <c r="P67" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="21">
+        <v>0</v>
+      </c>
+      <c r="R67" s="21">
+        <v>0</v>
+      </c>
+      <c r="S67" s="21">
+        <v>0</v>
+      </c>
+      <c r="T67" s="21">
+        <v>0</v>
+      </c>
+      <c r="U67" s="21">
+        <v>0</v>
+      </c>
+      <c r="V67" s="21">
+        <v>0</v>
+      </c>
+      <c r="W67" s="21">
+        <v>0</v>
+      </c>
+      <c r="X67" s="21">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="21">
+        <v>0</v>
+      </c>
       <c r="AB67" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:28" ht="15.75">
+      <c r="A68" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" s="8">
+        <v>30</v>
+      </c>
+      <c r="C68" s="8">
+        <v>3073</v>
+      </c>
+      <c r="D68" s="8">
+        <v>0</v>
+      </c>
+      <c r="E68" s="8">
+        <v>0</v>
+      </c>
+      <c r="F68" s="8">
+        <v>0</v>
+      </c>
+      <c r="G68" s="8">
+        <v>10</v>
+      </c>
+      <c r="H68" s="8">
+        <v>5</v>
+      </c>
+      <c r="I68" s="8">
+        <v>5</v>
+      </c>
+      <c r="J68" s="8">
+        <v>0</v>
+      </c>
+      <c r="K68" s="8">
+        <v>0</v>
+      </c>
+      <c r="L68" s="8">
+        <v>0</v>
+      </c>
+      <c r="M68" s="8">
+        <v>0</v>
+      </c>
+      <c r="N68" s="20">
+        <v>0</v>
+      </c>
+      <c r="O68" s="21">
+        <v>0</v>
+      </c>
+      <c r="P68" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="21">
+        <v>0</v>
+      </c>
+      <c r="R68" s="21">
+        <v>0</v>
+      </c>
+      <c r="S68" s="21">
+        <v>0</v>
+      </c>
+      <c r="T68" s="21">
+        <v>0</v>
+      </c>
+      <c r="U68" s="21">
+        <v>0</v>
+      </c>
+      <c r="V68" s="21">
+        <v>0</v>
+      </c>
+      <c r="W68" s="21">
+        <v>0</v>
+      </c>
+      <c r="X68" s="21">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="21">
+        <v>400</v>
+      </c>
       <c r="AB68" s="2">
-        <f>($D$2*D68)+($E$2*E68)+($F$2*F68)+($G$2*G68)+($H$2*H68)+($I$2*I68)+($J$2*J68)+($K$2*K68)+($L$2*L68)+($M$2*M68)+($N$2*N68)+($O$2*O68)+($P$2*P68)+($Q$2*Q68)+($R$2*R68)+($S$2*S68)+($T$2*T68)+($U$2*U68)+($V$2*V68)+($W$2*W68)+($X$2*X68)+($Y$2*Y68)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>925</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="15.75">
@@ -5792,8 +6081,8 @@
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:AC1048576 C135:C1048576 C3:C73 A3:B1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C73">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Item Tree + Hair of Samson
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -319,6 +319,15 @@
   </si>
   <si>
     <t>item_golden_fleece</t>
+  </si>
+  <si>
+    <t>item_recipe_hair_of_samson</t>
+  </si>
+  <si>
+    <t>item_hair_of_samson</t>
+  </si>
+  <si>
+    <t>components</t>
   </si>
 </sst>
 </file>
@@ -583,18 +592,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -608,37 +617,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -917,7 +896,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -927,9 +906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1590" topLeftCell="A40" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
+      <selection pane="bottomLeft" activeCell="AD70" sqref="AD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -962,37 +941,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="6" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
     </row>
     <row r="2" spans="1:29" s="7" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="7" t="s">
@@ -1066,37 +1045,37 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="16.5" thickTop="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
     </row>
     <row r="4" spans="1:29" ht="30">
       <c r="A4" s="1" t="s">
@@ -5709,7 +5688,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="15.75">
+    <row r="65" spans="1:29" ht="15.75">
       <c r="A65" t="s">
         <v>96</v>
       </c>
@@ -5793,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="15.75">
+    <row r="66" spans="1:29" ht="15.75">
       <c r="A66" s="12" t="s">
         <v>97</v>
       </c>
@@ -5836,40 +5815,40 @@
       <c r="N66" s="8">
         <v>0</v>
       </c>
-      <c r="O66" s="20">
-        <v>0</v>
-      </c>
-      <c r="P66" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q66" s="21">
-        <v>0</v>
-      </c>
-      <c r="R66" s="21">
-        <v>0</v>
-      </c>
-      <c r="S66" s="21">
-        <v>0</v>
-      </c>
-      <c r="T66" s="21">
-        <v>0</v>
-      </c>
-      <c r="U66" s="21">
-        <v>0</v>
-      </c>
-      <c r="V66" s="21">
-        <v>0</v>
-      </c>
-      <c r="W66" s="21">
-        <v>0</v>
-      </c>
-      <c r="X66" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="21">
+      <c r="O66" s="17">
+        <v>0</v>
+      </c>
+      <c r="P66" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="18">
+        <v>0</v>
+      </c>
+      <c r="R66" s="18">
+        <v>0</v>
+      </c>
+      <c r="S66" s="18">
+        <v>0</v>
+      </c>
+      <c r="T66" s="18">
+        <v>0</v>
+      </c>
+      <c r="U66" s="18">
+        <v>0</v>
+      </c>
+      <c r="V66" s="18">
+        <v>0</v>
+      </c>
+      <c r="W66" s="18">
+        <v>0</v>
+      </c>
+      <c r="X66" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="18">
         <v>0</v>
       </c>
       <c r="AA66">
@@ -5881,7 +5860,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="15.75">
+    <row r="67" spans="1:29" ht="15.75">
       <c r="A67" s="12" t="s">
         <v>98</v>
       </c>
@@ -5921,46 +5900,46 @@
       <c r="M67" s="8">
         <v>0</v>
       </c>
-      <c r="N67" s="20">
-        <v>0</v>
-      </c>
-      <c r="O67" s="21">
-        <v>0</v>
-      </c>
-      <c r="P67" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="21">
-        <v>0</v>
-      </c>
-      <c r="R67" s="21">
-        <v>0</v>
-      </c>
-      <c r="S67" s="21">
-        <v>0</v>
-      </c>
-      <c r="T67" s="21">
-        <v>0</v>
-      </c>
-      <c r="U67" s="21">
-        <v>0</v>
-      </c>
-      <c r="V67" s="21">
-        <v>0</v>
-      </c>
-      <c r="W67" s="21">
-        <v>0</v>
-      </c>
-      <c r="X67" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y67" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z67" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA67" s="21">
+      <c r="N67" s="17">
+        <v>0</v>
+      </c>
+      <c r="O67" s="18">
+        <v>0</v>
+      </c>
+      <c r="P67" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="18">
+        <v>0</v>
+      </c>
+      <c r="R67" s="18">
+        <v>0</v>
+      </c>
+      <c r="S67" s="18">
+        <v>0</v>
+      </c>
+      <c r="T67" s="18">
+        <v>0</v>
+      </c>
+      <c r="U67" s="18">
+        <v>0</v>
+      </c>
+      <c r="V67" s="18">
+        <v>0</v>
+      </c>
+      <c r="W67" s="18">
+        <v>0</v>
+      </c>
+      <c r="X67" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="18">
         <v>0</v>
       </c>
       <c r="AB67" s="2">
@@ -5968,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="15.75">
+    <row r="68" spans="1:29" ht="15.75">
       <c r="A68" s="12" t="s">
         <v>99</v>
       </c>
@@ -6008,43 +5987,43 @@
       <c r="M68" s="8">
         <v>0</v>
       </c>
-      <c r="N68" s="20">
-        <v>0</v>
-      </c>
-      <c r="O68" s="21">
-        <v>0</v>
-      </c>
-      <c r="P68" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q68" s="21">
-        <v>0</v>
-      </c>
-      <c r="R68" s="21">
-        <v>0</v>
-      </c>
-      <c r="S68" s="21">
-        <v>0</v>
-      </c>
-      <c r="T68" s="21">
-        <v>0</v>
-      </c>
-      <c r="U68" s="21">
-        <v>0</v>
-      </c>
-      <c r="V68" s="21">
-        <v>0</v>
-      </c>
-      <c r="W68" s="21">
-        <v>0</v>
-      </c>
-      <c r="X68" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y68" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z68" s="21">
+      <c r="N68" s="17">
+        <v>0</v>
+      </c>
+      <c r="O68" s="18">
+        <v>0</v>
+      </c>
+      <c r="P68" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="18">
+        <v>0</v>
+      </c>
+      <c r="R68" s="18">
+        <v>0</v>
+      </c>
+      <c r="S68" s="18">
+        <v>0</v>
+      </c>
+      <c r="T68" s="18">
+        <v>0</v>
+      </c>
+      <c r="U68" s="18">
+        <v>0</v>
+      </c>
+      <c r="V68" s="18">
+        <v>0</v>
+      </c>
+      <c r="W68" s="18">
+        <v>0</v>
+      </c>
+      <c r="X68" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="18">
         <v>400</v>
       </c>
       <c r="AB68" s="2">
@@ -6052,25 +6031,115 @@
         <v>925</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="15.75">
+    <row r="69" spans="1:29" ht="15.75">
+      <c r="A69" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C69" s="8">
+        <v>3074</v>
+      </c>
       <c r="AB69" s="2">
         <f>($D$2*D69)+($E$2*E69)+($F$2*F69)+($G$2*G69)+($H$2*H69)+($I$2*I69)+($J$2*J69)+($K$2*K69)+($L$2*L69)+($M$2*M69)+($N$2*N69)+($O$2*O69)+($P$2*P69)+($Q$2*Q69)+($R$2*R69)+($S$2*S69)+($T$2*T69)+($U$2*U69)+($V$2*V69)+($W$2*W69)+($X$2*X69)+($Y$2*Y69)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="15.75">
+    <row r="70" spans="1:29" ht="15.75">
+      <c r="A70" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="8">
+        <v>30</v>
+      </c>
+      <c r="C70" s="8">
+        <v>3075</v>
+      </c>
+      <c r="D70" s="17">
+        <v>0</v>
+      </c>
+      <c r="E70" s="18">
+        <v>0</v>
+      </c>
+      <c r="F70" s="18">
+        <v>6</v>
+      </c>
+      <c r="G70" s="18">
+        <v>0</v>
+      </c>
+      <c r="H70" s="18">
+        <v>0</v>
+      </c>
+      <c r="I70" s="18">
+        <v>0</v>
+      </c>
+      <c r="J70" s="18">
+        <v>0</v>
+      </c>
+      <c r="K70" s="18">
+        <v>0</v>
+      </c>
+      <c r="L70" s="18">
+        <v>0</v>
+      </c>
+      <c r="M70" s="18">
+        <v>0</v>
+      </c>
+      <c r="N70" s="18">
+        <v>0</v>
+      </c>
+      <c r="O70" s="18">
+        <v>0</v>
+      </c>
+      <c r="P70" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="18">
+        <v>0</v>
+      </c>
+      <c r="R70" s="18">
+        <v>0</v>
+      </c>
+      <c r="S70" s="18">
+        <v>0</v>
+      </c>
+      <c r="T70" s="18">
+        <v>0</v>
+      </c>
+      <c r="U70" s="18">
+        <v>0</v>
+      </c>
+      <c r="V70" s="18">
+        <v>0</v>
+      </c>
+      <c r="W70" s="18">
+        <v>0</v>
+      </c>
+      <c r="X70" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y70" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="18">
+        <v>0</v>
+      </c>
       <c r="AB70" s="2">
         <f>($D$2*D70)+($E$2*E70)+($F$2*F70)+($G$2*G70)+($H$2*H70)+($I$2*I70)+($J$2*J70)+($K$2*K70)+($L$2*L70)+($M$2*M70)+($N$2*N70)+($O$2*O70)+($P$2*P70)+($Q$2*Q70)+($R$2*R70)+($S$2*S70)+($T$2*T70)+($U$2*U70)+($V$2*V70)+($W$2*W70)+($X$2*X70)+($Y$2*Y70)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:28" ht="15.75">
+        <v>300</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" ht="15.75">
       <c r="AB71" s="2">
         <f t="shared" ref="AB71:AB72" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="15.75">
+    <row r="72" spans="1:29" ht="15.75">
       <c r="AB72" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6082,7 +6151,7 @@
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C73">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
item work + caduceus
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -334,6 +334,18 @@
   </si>
   <si>
     <t>item_war_belt</t>
+  </si>
+  <si>
+    <t>item_recipe_caduceus</t>
+  </si>
+  <si>
+    <t>item_caduceus</t>
+  </si>
+  <si>
+    <t>item_recipe_zoster_of_hippolyta</t>
+  </si>
+  <si>
+    <t>item_zoster_of_hippolyta</t>
   </si>
 </sst>
 </file>
@@ -623,7 +635,57 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -902,7 +964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -910,11 +972,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC72"/>
+  <dimension ref="A1:AC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1590" topLeftCell="A40" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <pane ySplit="1590" topLeftCell="A43" activePane="bottomLeft"/>
+      <selection activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6222,7 +6285,7 @@
         <v>0</v>
       </c>
       <c r="AB71" s="2">
-        <f t="shared" ref="AB71:AB72" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
+        <f t="shared" ref="AB71:AB76" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
         <v>0</v>
       </c>
       <c r="AC71" t="s">
@@ -6317,6 +6380,163 @@
       </c>
       <c r="AC72" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" ht="15.75">
+      <c r="A73" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C73" s="8">
+        <v>3078</v>
+      </c>
+      <c r="AB73" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" ht="15.75">
+      <c r="A74" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" s="8">
+        <v>30</v>
+      </c>
+      <c r="C74" s="8">
+        <v>3079</v>
+      </c>
+      <c r="D74" s="17">
+        <v>0</v>
+      </c>
+      <c r="E74" s="18">
+        <v>0</v>
+      </c>
+      <c r="F74" s="18">
+        <v>0</v>
+      </c>
+      <c r="G74" s="18">
+        <v>20</v>
+      </c>
+      <c r="H74" s="18">
+        <v>0</v>
+      </c>
+      <c r="I74" s="18">
+        <v>0</v>
+      </c>
+      <c r="J74" s="18">
+        <v>0</v>
+      </c>
+      <c r="K74" s="18">
+        <v>0</v>
+      </c>
+      <c r="L74" s="18">
+        <v>0</v>
+      </c>
+      <c r="M74" s="18">
+        <v>0</v>
+      </c>
+      <c r="N74" s="18">
+        <v>0</v>
+      </c>
+      <c r="O74" s="18">
+        <v>0</v>
+      </c>
+      <c r="P74" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="18">
+        <v>0</v>
+      </c>
+      <c r="R74" s="18">
+        <v>0</v>
+      </c>
+      <c r="S74" s="18">
+        <v>0</v>
+      </c>
+      <c r="T74" s="18">
+        <v>0</v>
+      </c>
+      <c r="U74" s="18">
+        <v>0</v>
+      </c>
+      <c r="V74" s="18">
+        <v>0</v>
+      </c>
+      <c r="W74" s="18">
+        <v>0</v>
+      </c>
+      <c r="X74" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y74" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA74" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB74" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="AC74" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" ht="15.75">
+      <c r="A75" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C75" s="8">
+        <v>3080</v>
+      </c>
+      <c r="AB75" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" ht="15.75">
+      <c r="A76" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="8">
+        <v>2</v>
+      </c>
+      <c r="C76" s="8">
+        <v>3081</v>
+      </c>
+      <c r="F76" s="18">
+        <v>10</v>
+      </c>
+      <c r="G76" s="18">
+        <v>30</v>
+      </c>
+      <c r="H76" s="18">
+        <v>5</v>
+      </c>
+      <c r="I76" s="18">
+        <v>5</v>
+      </c>
+      <c r="Z76" s="18">
+        <v>400</v>
+      </c>
+      <c r="AA76">
+        <f>AB68+AB70+AB72+AB74</f>
+        <v>1575</v>
+      </c>
+      <c r="AB76" s="2">
+        <f t="shared" si="1"/>
+        <v>1225</v>
       </c>
     </row>
   </sheetData>
@@ -6324,8 +6544,8 @@
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C73">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C76 D3:AC1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Item - Wooden Shield [WIP]
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -10,16 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -352,6 +348,12 @@
   </si>
   <si>
     <t>item_greater_agility</t>
+  </si>
+  <si>
+    <t>item_recipe_wooden_shield</t>
+  </si>
+  <si>
+    <t>item_wooden_shield</t>
   </si>
 </sst>
 </file>
@@ -684,14 +686,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -950,7 +944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -958,12 +952,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC78"/>
+  <dimension ref="A1:AC80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1590" topLeftCell="A43" activePane="bottomLeft"/>
-      <selection activeCell="D2" sqref="D2"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76:XFD76"/>
+      <pane ySplit="1590" topLeftCell="A52" activePane="bottomLeft"/>
+      <selection activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1060,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="M2" s="7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N2" s="7">
         <v>10</v>
@@ -2366,7 +2360,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="AC20" s="2" t="s">
         <v>15</v>
@@ -6271,7 +6265,7 @@
         <v>0</v>
       </c>
       <c r="AB71" s="2">
-        <f t="shared" ref="AB71:AB78" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
+        <f t="shared" ref="AB71:AB80" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
         <v>0</v>
       </c>
       <c r="AC71" t="s">
@@ -6631,6 +6625,45 @@
       </c>
       <c r="AC78" s="12" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" ht="15.75">
+      <c r="A79" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C79" s="8">
+        <v>3084</v>
+      </c>
+      <c r="AB79" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC79" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" ht="15.75">
+      <c r="A80" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="8">
+        <v>3</v>
+      </c>
+      <c r="C80" s="8">
+        <v>3085</v>
+      </c>
+      <c r="M80">
+        <v>10</v>
+      </c>
+      <c r="AB80" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -6638,7 +6671,7 @@
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C78 D3:AC1048576">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C80 D3:AC1048576">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Consumables and Publish Assets
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -354,6 +353,15 @@
   </si>
   <si>
     <t>item_wooden_shield</t>
+  </si>
+  <si>
+    <t>item_ambrosia</t>
+  </si>
+  <si>
+    <t>item_health_potion</t>
+  </si>
+  <si>
+    <t>item_mana_potion</t>
   </si>
 </sst>
 </file>
@@ -944,7 +952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -952,12 +960,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC80"/>
+  <dimension ref="A1:AC83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1590" topLeftCell="A52" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M2"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6666,12 +6674,45 @@
         <v>15</v>
       </c>
     </row>
+    <row r="81" spans="1:3" ht="15.75">
+      <c r="A81" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" s="8">
+        <v>16</v>
+      </c>
+      <c r="C81" s="8">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75">
+      <c r="A82" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B82" s="8">
+        <v>16</v>
+      </c>
+      <c r="C82" s="8">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75">
+      <c r="A83" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B83" s="8">
+        <v>16</v>
+      </c>
+      <c r="C83" s="8">
+        <v>3088</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C80 D3:AC1048576">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C83">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
mana potion and fixing multiplayer spawn bugs
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -651,7 +651,57 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -962,10 +1012,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1590" topLeftCell="A52" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1590" topLeftCell="A61" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M2"/>
-      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
+      <selection pane="bottomLeft" activeCell="AA82" sqref="AA82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1431,7 +1481,7 @@
       </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2">
-        <f t="shared" ref="AB7:AB68" si="0">($D$2*D7)+($E$2*E7)+($F$2*F7)+($G$2*G7)+($H$2*H7)+($I$2*I7)+($J$2*J7)+($K$2*K7)+($L$2*L7)+($M$2*M7)+($N$2*N7)+($O$2*O7)+($P$2*P7)+($Q$2*Q7)+($R$2*R7)+($S$2*S7)+($T$2*T7)+($U$2*U7)+($V$2*V7)+($W$2*W7)+($X$2*X7)+($Y$2*Y7)+($Z$2*Z7)+(AA7)</f>
+        <f t="shared" ref="AB7:AB70" si="0">($D$2*D7)+($E$2*E7)+($F$2*F7)+($G$2*G7)+($H$2*H7)+($I$2*I7)+($J$2*J7)+($K$2*K7)+($L$2*L7)+($M$2*M7)+($N$2*N7)+($O$2*O7)+($P$2*P7)+($Q$2*Q7)+($R$2*R7)+($S$2*S7)+($T$2*T7)+($U$2*U7)+($V$2*V7)+($W$2*W7)+($X$2*X7)+($Y$2*Y7)+($Z$2*Z7)+(AA7)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="2" t="s">
@@ -4615,7 +4665,7 @@
       </c>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2">
-        <f t="shared" si="0"/>
+        <f>($D$2*D51)+($E$2*E51)+($F$2*F51)+($G$2*G51)+($H$2*H51)+($I$2*I51)+($J$2*J51)+($K$2*K51)+($L$2*L51)+($M$2*M51)+($N$2*N51)+($O$2*O51)+($P$2*P51)+($Q$2*Q51)+($R$2*R51)+($S$2*S51)+($T$2*T51)+($U$2*U51)+($V$2*V51)+($W$2*W51)+($X$2*X51)+($Y$2*Y51)+($Z$2*Z51)+(AA51)</f>
         <v>0</v>
       </c>
       <c r="AC51" s="8" t="s">
@@ -6099,7 +6149,7 @@
         <v>3074</v>
       </c>
       <c r="AB69" s="2">
-        <f>($D$2*D69)+($E$2*E69)+($F$2*F69)+($G$2*G69)+($H$2*H69)+($I$2*I69)+($J$2*J69)+($K$2*K69)+($L$2*L69)+($M$2*M69)+($N$2*N69)+($O$2*O69)+($P$2*P69)+($Q$2*Q69)+($R$2*R69)+($S$2*S69)+($T$2*T69)+($U$2*U69)+($V$2*V69)+($W$2*W69)+($X$2*X69)+($Y$2*Y69)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6183,7 +6233,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="2">
-        <f>($D$2*D70)+($E$2*E70)+($F$2*F70)+($G$2*G70)+($H$2*H70)+($I$2*I70)+($J$2*J70)+($K$2*K70)+($L$2*L70)+($M$2*M70)+($N$2*N70)+($O$2*O70)+($P$2*P70)+($Q$2*Q70)+($R$2*R70)+($S$2*S70)+($T$2*T70)+($U$2*U70)+($V$2*V70)+($W$2*W70)+($X$2*X70)+($Y$2*Y70)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="AC70" t="s">
@@ -6273,7 +6323,7 @@
         <v>0</v>
       </c>
       <c r="AB71" s="2">
-        <f t="shared" ref="AB71:AB80" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)</f>
+        <f t="shared" ref="AB71:AB80" si="1">($D$2*D71)+($E$2*E71)+($F$2*F71)+($G$2*G71)+($H$2*H71)+($I$2*I71)+($J$2*J71)+($K$2*K71)+($L$2*L71)+($M$2*M71)+($N$2*N71)+($O$2*O71)+($P$2*P71)+($Q$2*Q71)+($R$2*R71)+($S$2*S71)+($T$2*T71)+($U$2*U71)+($V$2*V71)+($W$2*W71)+($X$2*X71)+($Y$2*Y71)+($Z$2*Z71)+(AA71)</f>
         <v>0</v>
       </c>
       <c r="AC71" t="s">
@@ -6524,7 +6574,7 @@
       </c>
       <c r="AB76" s="2">
         <f t="shared" si="1"/>
-        <v>1225</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="77" spans="1:29" ht="15.75">
@@ -6674,7 +6724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75">
+    <row r="81" spans="1:29" ht="15.75">
       <c r="A81" s="12" t="s">
         <v>113</v>
       </c>
@@ -6684,8 +6734,18 @@
       <c r="C81" s="8">
         <v>3086</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75">
+      <c r="Z81">
+        <v>200</v>
+      </c>
+      <c r="AB81" s="2">
+        <f>($D$2*D81)+($E$2*E81)+($F$2*F81)+($G$2*G81)+($H$2*H81)+($I$2*I81)+($J$2*J81)+($K$2*K81)+($L$2*L81)+($M$2*M81)+($N$2*N81)+($O$2*O81)+($P$2*P81)+($Q$2*Q81)+($R$2*R81)+($S$2*S81)+($T$2*T81)+($U$2*U81)+($V$2*V81)+($W$2*W81)+($X$2*X81)+($Y$2*Y81)+($Z$2*Z81)+(AA81)</f>
+        <v>200</v>
+      </c>
+      <c r="AC81" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" ht="15.75">
       <c r="A82" s="12" t="s">
         <v>114</v>
       </c>
@@ -6695,8 +6755,18 @@
       <c r="C82" s="8">
         <v>3087</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75">
+      <c r="Z82">
+        <v>100</v>
+      </c>
+      <c r="AB82" s="2">
+        <f t="shared" ref="AB82:AB83" si="2">($D$2*D82)+($E$2*E82)+($F$2*F82)+($G$2*G82)+($H$2*H82)+($I$2*I82)+($J$2*J82)+($K$2*K82)+($L$2*L82)+($M$2*M82)+($N$2*N82)+($O$2*O82)+($P$2*P82)+($Q$2*Q82)+($R$2*R82)+($S$2*S82)+($T$2*T82)+($U$2*U82)+($V$2*V82)+($W$2*W82)+($X$2*X82)+($Y$2*Y82)+($Z$2*Z82)+(AA82)</f>
+        <v>100</v>
+      </c>
+      <c r="AC82" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" ht="15.75">
       <c r="A83" s="12" t="s">
         <v>115</v>
       </c>
@@ -6705,6 +6775,16 @@
       </c>
       <c r="C83" s="8">
         <v>3088</v>
+      </c>
+      <c r="Z83">
+        <v>50</v>
+      </c>
+      <c r="AB83" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="AC83" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -6712,8 +6792,8 @@
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C83">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C83 D3:AC1048576">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Merc Spawn Fixes, Item Models, and Working on Obs/Sents
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>item_mana_potion</t>
+  </si>
+  <si>
+    <t>item_eye_of_argus</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -1010,12 +1023,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC83"/>
+  <dimension ref="A1:AC84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1590" topLeftCell="A61" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M2"/>
-      <selection pane="bottomLeft" activeCell="AA82" sqref="AA82"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6787,13 +6800,24 @@
         <v>62</v>
       </c>
     </row>
+    <row r="84" spans="1:29" ht="15.75">
+      <c r="A84" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B84" s="8">
+        <v>5</v>
+      </c>
+      <c r="C84" s="8">
+        <v>3089</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C83 D3:AC1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C84">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Item - Carnyx + trying to get backpack to display full color
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\avalore\balancing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D99DD6-3492-4D44-A199-63B4E5BACE5B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -365,12 +372,18 @@
   </si>
   <si>
     <t>item_eye_of_argus</t>
+  </si>
+  <si>
+    <t>item_recipe_carnyx</t>
+  </si>
+  <si>
+    <t>item_carnyx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -654,97 +667,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="1" tint="0.499984740745262"/>
@@ -757,6 +680,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1015,20 +946,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1590" topLeftCell="A61" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M2"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1164,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="16.5" thickTop="1">
+    <row r="3" spans="1:29" ht="15.75" thickTop="1">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -1286,7 +1217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75">
+    <row r="5" spans="1:29">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1357,7 +1288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75">
+    <row r="6" spans="1:29">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75">
+    <row r="7" spans="1:29">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1501,7 +1432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15.75">
+    <row r="8" spans="1:29">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1573,7 +1504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75">
+    <row r="9" spans="1:29">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15.75">
+    <row r="10" spans="1:29">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15.75">
+    <row r="11" spans="1:29">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1789,7 +1720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.75">
+    <row r="12" spans="1:29">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1861,7 +1792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15.75">
+    <row r="13" spans="1:29">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1933,7 +1864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15.75">
+    <row r="14" spans="1:29">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -2005,7 +1936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75">
+    <row r="15" spans="1:29">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -2077,7 +2008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75">
+    <row r="16" spans="1:29">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -2149,7 +2080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="15.75">
+    <row r="17" spans="1:29">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -2221,7 +2152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="15.75">
+    <row r="18" spans="1:29">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -2293,7 +2224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15.75">
+    <row r="19" spans="1:29">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -2365,7 +2296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15.75">
+    <row r="20" spans="1:29">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -2437,7 +2368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15.75">
+    <row r="21" spans="1:29">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
@@ -2509,7 +2440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="15.75">
+    <row r="22" spans="1:29">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -2581,7 +2512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="15.75">
+    <row r="23" spans="1:29">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -2653,7 +2584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="15.75">
+    <row r="24" spans="1:29">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -2725,7 +2656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="15.75">
+    <row r="25" spans="1:29">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -2797,7 +2728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="15.75">
+    <row r="26" spans="1:29">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -2869,7 +2800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="15.75">
+    <row r="27" spans="1:29">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -2941,7 +2872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75">
+    <row r="28" spans="1:29">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -3013,7 +2944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="15.75">
+    <row r="29" spans="1:29">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
@@ -3085,7 +3016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="15.75">
+    <row r="30" spans="1:29">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
@@ -3157,7 +3088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="15.75">
+    <row r="31" spans="1:29">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -3229,7 +3160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="15.75">
+    <row r="32" spans="1:29">
       <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
@@ -3301,7 +3232,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="15.75">
+    <row r="33" spans="1:29">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -3373,7 +3304,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="15.75">
+    <row r="34" spans="1:29">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
@@ -3445,7 +3376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="15.75">
+    <row r="35" spans="1:29">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -3517,7 +3448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="15.75">
+    <row r="36" spans="1:29">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
@@ -3589,7 +3520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="15.75">
+    <row r="37" spans="1:29">
       <c r="A37" s="2" t="s">
         <v>48</v>
       </c>
@@ -3661,7 +3592,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="15.75">
+    <row r="38" spans="1:29">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
@@ -3733,7 +3664,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="15.75">
+    <row r="39" spans="1:29">
       <c r="A39" s="2" t="s">
         <v>50</v>
       </c>
@@ -3805,7 +3736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="15.75">
+    <row r="40" spans="1:29">
       <c r="A40" s="2" t="s">
         <v>51</v>
       </c>
@@ -3877,7 +3808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="15.75">
+    <row r="41" spans="1:29">
       <c r="A41" s="2" t="s">
         <v>52</v>
       </c>
@@ -3949,7 +3880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="15.75">
+    <row r="42" spans="1:29">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -4021,7 +3952,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="15.75">
+    <row r="43" spans="1:29">
       <c r="A43" s="2" t="s">
         <v>54</v>
       </c>
@@ -4093,7 +4024,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="15.75">
+    <row r="44" spans="1:29">
       <c r="A44" s="2" t="s">
         <v>56</v>
       </c>
@@ -4165,7 +4096,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="15.75">
+    <row r="45" spans="1:29">
       <c r="A45" s="2" t="s">
         <v>57</v>
       </c>
@@ -4237,7 +4168,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="15.75">
+    <row r="46" spans="1:29">
       <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
@@ -4309,7 +4240,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="15.75">
+    <row r="47" spans="1:29">
       <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
@@ -4381,7 +4312,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="15.75">
+    <row r="48" spans="1:29">
       <c r="A48" s="2" t="s">
         <v>60</v>
       </c>
@@ -4453,7 +4384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:29" ht="15.75">
+    <row r="49" spans="1:29">
       <c r="A49" s="2" t="s">
         <v>61</v>
       </c>
@@ -4525,7 +4456,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="15.75">
+    <row r="50" spans="1:29">
       <c r="A50" s="2" t="s">
         <v>63</v>
       </c>
@@ -4597,7 +4528,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="15.75">
+    <row r="51" spans="1:29">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -4685,7 +4616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="15.75">
+    <row r="52" spans="1:29">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -4773,7 +4704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="15.75">
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -4861,7 +4792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:29" ht="15.75">
+    <row r="54" spans="1:29">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -4949,7 +4880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="15.75">
+    <row r="55" spans="1:29">
       <c r="A55" t="s">
         <v>81</v>
       </c>
@@ -5037,7 +4968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="15.75">
+    <row r="56" spans="1:29">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -5125,7 +5056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="15.75">
+    <row r="57" spans="1:29">
       <c r="A57" t="s">
         <v>83</v>
       </c>
@@ -5210,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:29" s="11" customFormat="1" ht="15.75">
+    <row r="58" spans="1:29" s="11" customFormat="1">
       <c r="A58" s="11" t="s">
         <v>84</v>
       </c>
@@ -5295,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="15.75">
+    <row r="59" spans="1:29">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -5380,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="15.75">
+    <row r="60" spans="1:29">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -5465,7 +5396,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="61" spans="1:29" ht="15.75">
+    <row r="61" spans="1:29">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -5550,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="15.75">
+    <row r="62" spans="1:29">
       <c r="A62" s="12" t="s">
         <v>88</v>
       </c>
@@ -5638,7 +5569,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="15.75">
+    <row r="63" spans="1:29">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -5723,7 +5654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="15.75">
+    <row r="64" spans="1:29">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -5808,7 +5739,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="65" spans="1:29" ht="15.75">
+    <row r="65" spans="1:29">
       <c r="A65" t="s">
         <v>96</v>
       </c>
@@ -5892,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="15.75">
+    <row r="66" spans="1:29">
       <c r="A66" s="12" t="s">
         <v>97</v>
       </c>
@@ -5980,7 +5911,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="15.75">
+    <row r="67" spans="1:29">
       <c r="A67" s="12" t="s">
         <v>98</v>
       </c>
@@ -6067,7 +5998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="15.75">
+    <row r="68" spans="1:29">
       <c r="A68" s="12" t="s">
         <v>99</v>
       </c>
@@ -6151,7 +6082,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="15.75">
+    <row r="69" spans="1:29">
       <c r="A69" s="12" t="s">
         <v>100</v>
       </c>
@@ -6166,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="15.75">
+    <row r="70" spans="1:29">
       <c r="A70" s="12" t="s">
         <v>101</v>
       </c>
@@ -6253,7 +6184,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="15.75">
+    <row r="71" spans="1:29">
       <c r="A71" s="12" t="s">
         <v>103</v>
       </c>
@@ -6343,7 +6274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="15.75">
+    <row r="72" spans="1:29">
       <c r="A72" s="12" t="s">
         <v>104</v>
       </c>
@@ -6433,7 +6364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="15.75">
+    <row r="73" spans="1:29">
       <c r="A73" s="12" t="s">
         <v>105</v>
       </c>
@@ -6451,7 +6382,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="15.75">
+    <row r="74" spans="1:29">
       <c r="A74" s="12" t="s">
         <v>106</v>
       </c>
@@ -6541,7 +6472,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:29" ht="15.75">
+    <row r="75" spans="1:29">
       <c r="A75" s="12" t="s">
         <v>107</v>
       </c>
@@ -6556,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="15.75">
+    <row r="76" spans="1:29">
       <c r="A76" s="12" t="s">
         <v>108</v>
       </c>
@@ -6590,7 +6521,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="77" spans="1:29" ht="15.75">
+    <row r="77" spans="1:29">
       <c r="A77" s="12" t="s">
         <v>109</v>
       </c>
@@ -6608,7 +6539,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:29" ht="15.75">
+    <row r="78" spans="1:29">
       <c r="A78" s="12" t="s">
         <v>110</v>
       </c>
@@ -6698,7 +6629,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:29" ht="15.75">
+    <row r="79" spans="1:29">
       <c r="A79" s="12" t="s">
         <v>111</v>
       </c>
@@ -6716,7 +6647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:29" ht="15.75">
+    <row r="80" spans="1:29">
       <c r="A80" s="12" t="s">
         <v>112</v>
       </c>
@@ -6737,7 +6668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:29" ht="15.75">
+    <row r="81" spans="1:29">
       <c r="A81" s="12" t="s">
         <v>113</v>
       </c>
@@ -6758,7 +6689,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="15.75">
+    <row r="82" spans="1:29">
       <c r="A82" s="12" t="s">
         <v>114</v>
       </c>
@@ -6772,14 +6703,14 @@
         <v>100</v>
       </c>
       <c r="AB82" s="2">
-        <f t="shared" ref="AB82:AB83" si="2">($D$2*D82)+($E$2*E82)+($F$2*F82)+($G$2*G82)+($H$2*H82)+($I$2*I82)+($J$2*J82)+($K$2*K82)+($L$2*L82)+($M$2*M82)+($N$2*N82)+($O$2*O82)+($P$2*P82)+($Q$2*Q82)+($R$2*R82)+($S$2*S82)+($T$2*T82)+($U$2*U82)+($V$2*V82)+($W$2*W82)+($X$2*X82)+($Y$2*Y82)+($Z$2*Z82)+(AA82)</f>
+        <f t="shared" ref="AB82:AB88" si="2">($D$2*D82)+($E$2*E82)+($F$2*F82)+($G$2*G82)+($H$2*H82)+($I$2*I82)+($J$2*J82)+($K$2*K82)+($L$2*L82)+($M$2*M82)+($N$2*N82)+($O$2*O82)+($P$2*P82)+($Q$2*Q82)+($R$2*R82)+($S$2*S82)+($T$2*T82)+($U$2*U82)+($V$2*V82)+($W$2*W82)+($X$2*X82)+($Y$2*Y82)+($Z$2*Z82)+(AA82)</f>
         <v>100</v>
       </c>
       <c r="AC82" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="15.75">
+    <row r="83" spans="1:29">
       <c r="A83" s="12" t="s">
         <v>115</v>
       </c>
@@ -6800,7 +6731,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="15.75">
+    <row r="84" spans="1:29">
       <c r="A84" s="12" t="s">
         <v>116</v>
       </c>
@@ -6809,6 +6740,61 @@
       </c>
       <c r="C84" s="8">
         <v>3089</v>
+      </c>
+      <c r="AB84" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29">
+      <c r="A85" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B85" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C85" s="8">
+        <v>3090</v>
+      </c>
+      <c r="AB85" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29">
+      <c r="A86" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86" s="8">
+        <v>30</v>
+      </c>
+      <c r="C86" s="8">
+        <v>3091</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+      <c r="AB86" s="2">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29">
+      <c r="AB87" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29">
+      <c r="AB88" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6816,8 +6802,8 @@
     <mergeCell ref="A3:AC3"/>
     <mergeCell ref="A1:AC1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 D3:AC1048576 C3:C84">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+  <conditionalFormatting sqref="C135:C1048576 A3:B1048576 C3:C86 D3:AC1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[WIP] Items + Bugs
- added attack speed item
- fixed a bug where some backpacked items didn't show up in the HUD because the caster was a modifier not a player
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -383,6 +383,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_lesser_mana_regen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_lesser_attack_speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_lesser_attack_speed</t>
   </si>
 </sst>
 </file>
@@ -816,12 +822,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC88"/>
+  <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1590" topLeftCell="A67" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AB88" activeCellId="0" sqref="AB88"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K91" activeCellId="0" sqref="K91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6657,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>120</v>
       </c>
@@ -6670,6 +6676,51 @@
       <c r="AB88" s="14" t="n">
         <f aca="false">($D$2*D88)+($E$2*E88)+($F$2*F88)+($G$2*G88)+($H$2*H88)+($I$2*I88)+($J$2*J88)+($K$2*K88)+($L$2*L88)+($M$2*M88)+($N$2*N88)+($O$2*O88)+($P$2*P88)+($Q$2*Q88)+($R$2*R88)+($S$2*S88)+($T$2*T88)+($U$2*U88)+($V$2*V88)+($W$2*W88)+($X$2*X88)+($Y$2*Y88)+($Z$2*Z88)+(AA88)</f>
         <v>125</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB89" s="14" t="n">
+        <f aca="false">($D$2*D89)+($E$2*E89)+($F$2*F89)+($G$2*G89)+($H$2*H89)+($I$2*I89)+($J$2*J89)+($K$2*K89)+($L$2*L89)+($M$2*M89)+($N$2*N89)+($O$2*O89)+($P$2*P89)+($Q$2*Q89)+($R$2*R89)+($S$2*S89)+($T$2*T89)+($U$2*U89)+($V$2*V89)+($W$2*W89)+($X$2*X89)+($Y$2*Y89)+($Z$2*Z89)+(AA89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="H90" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AB90" s="14" t="n">
+        <f aca="false">($D$2*D90)+($E$2*E90)+($F$2*F90)+($G$2*G90)+($H$2*H90)+($I$2*I90)+($J$2*J90)+($K$2*K90)+($L$2*L90)+($M$2*M90)+($N$2*N90)+($O$2*O90)+($P$2*P90)+($Q$2*Q90)+($R$2*R90)+($S$2*S90)+($T$2*T90)+($U$2*U90)+($V$2*V90)+($W$2*W90)+($X$2*X90)+($Y$2*Y90)+($Z$2*Z90)+(AA90)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB91" s="14" t="n">
+        <f aca="false">($D$2*D91)+($E$2*E91)+($F$2*F91)+($G$2*G91)+($H$2*H91)+($I$2*I91)+($J$2*J91)+($K$2*K91)+($L$2*L91)+($M$2*M91)+($N$2*N91)+($O$2*O91)+($P$2*P91)+($Q$2*Q91)+($R$2*R91)+($S$2*S91)+($T$2*T91)+($U$2*U91)+($V$2*V91)+($W$2*W91)+($X$2*X91)+($Y$2*Y91)+($Z$2*Z91)+(AA91)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB92" s="14" t="n">
+        <f aca="false">($D$2*D92)+($E$2*E92)+($F$2*F92)+($G$2*G92)+($H$2*H92)+($I$2*I92)+($J$2*J92)+($K$2*K92)+($L$2*L92)+($M$2*M92)+($N$2*N92)+($O$2*O92)+($P$2*P92)+($Q$2*Q92)+($R$2*R92)+($S$2*S92)+($T$2*T92)+($U$2*U92)+($V$2*V92)+($W$2*W92)+($X$2*X92)+($Y$2*Y92)+($Z$2*Z92)+(AA92)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB93" s="14" t="n">
+        <f aca="false">($D$2*D93)+($E$2*E93)+($F$2*F93)+($G$2*G93)+($H$2*H93)+($I$2*I93)+($J$2*J93)+($K$2*K93)+($L$2*L93)+($M$2*M93)+($N$2*N93)+($O$2*O93)+($P$2*P93)+($Q$2*Q93)+($R$2*R93)+($S$2*S93)+($T$2*T93)+($U$2*U93)+($V$2*V93)+($W$2*W93)+($X$2*X93)+($Y$2*Y93)+($Z$2*Z93)+(AA93)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Item - War Belt [Rework]
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -815,7 +815,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C94" activeCellId="0" sqref="C94"/>
+      <selection pane="bottomLeft" activeCell="D72" activeCellId="0" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6146,7 +6146,7 @@
         <v>3077</v>
       </c>
       <c r="D72" s="17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E72" s="17" t="n">
         <v>0</v>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="AB72" s="17" t="n">
         <f aca="false">($D$2*D72)+($E$2*E72)+($F$2*F72)+($G$2*G72)+($H$2*H72)+($I$2*I72)+($J$2*J72)+($K$2*K72)+($L$2*L72)+($M$2*M72)+($N$2*N72)+($O$2*O72)+($P$2*P72)+($Q$2*Q72)+($R$2*R72)+($S$2*S72)+($T$2*T72)+($U$2*U72)+($V$2*V72)+($W$2*W72)+($X$2*X72)+($Y$2*Y72)+($Z$2*Z72)+(AA72)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="AC72" s="1" t="s">
         <v>33</v>
@@ -6375,11 +6375,11 @@
       </c>
       <c r="AA76" s="1" t="n">
         <f aca="false">AB68+AB70+AB72+AB74+AB78</f>
-        <v>1875</v>
+        <v>2025</v>
       </c>
       <c r="AB76" s="17" t="n">
         <f aca="false">($D$2*D76)+($E$2*E76)+($F$2*F76)+($G$2*G76)+($H$2*H76)+($I$2*I76)+($J$2*J76)+($K$2*K76)+($L$2*L76)+($M$2*M76)+($N$2*N76)+($O$2*O76)+($P$2*P76)+($Q$2*Q76)+($R$2*R76)+($S$2*S76)+($T$2*T76)+($U$2*U76)+($V$2*V76)+($W$2*W76)+($X$2*X76)+($Y$2*Y76)+($Z$2*Z76)+(AA76)</f>
-        <v>3500</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Item - Zoster of Hippolyta [Rework]
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -815,7 +815,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D72" activeCellId="0" sqref="D72"/>
+      <selection pane="bottomLeft" activeCell="A76" activeCellId="0" sqref="76:76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6358,11 +6358,14 @@
       <c r="C76" s="18" t="n">
         <v>3081</v>
       </c>
+      <c r="D76" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="F76" s="17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G76" s="17" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H76" s="17" t="n">
         <v>5</v>
@@ -6379,7 +6382,7 @@
       </c>
       <c r="AB76" s="17" t="n">
         <f aca="false">($D$2*D76)+($E$2*E76)+($F$2*F76)+($G$2*G76)+($H$2*H76)+($I$2*I76)+($J$2*J76)+($K$2*K76)+($L$2*L76)+($M$2*M76)+($N$2*N76)+($O$2*O76)+($P$2*P76)+($Q$2*Q76)+($R$2*R76)+($S$2*S76)+($T$2*T76)+($U$2*U76)+($V$2*V76)+($W$2*W76)+($X$2*X76)+($Y$2*Y76)+($Z$2*Z76)+(AA76)</f>
-        <v>3650</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Item - Brunhild's Girdle
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="129">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -401,6 +401,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_bonemace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_brunhilds_girdle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_brunhilds_girdle</t>
   </si>
 </sst>
 </file>
@@ -812,10 +818,10 @@
   </sheetPr>
   <dimension ref="A1:AC100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A76" activeCellId="0" sqref="76:76"/>
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="AD98" activeCellId="0" sqref="AD98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6779,30 +6785,72 @@
       <c r="Z94" s="1" t="n">
         <v>1000</v>
       </c>
+      <c r="AB94" s="17" t="n">
+        <f aca="false">($D$2*D94)+($E$2*E94)+($F$2*F94)+($G$2*G94)+($H$2*H94)+($I$2*I94)+($J$2*J94)+($K$2*K94)+($L$2*L94)+($M$2*M94)+($N$2*N94)+($O$2*O94)+($P$2*P94)+($Q$2*Q94)+($R$2*R94)+($S$2*S94)+($T$2*T94)+($U$2*U94)+($V$2*V94)+($W$2*W94)+($X$2*X94)+($Y$2*Y94)+($Z$2*Z94)+(AA94)</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C95" s="18" t="n">
         <v>3100</v>
       </c>
+      <c r="AB95" s="17" t="n">
+        <f aca="false">($D$2*D95)+($E$2*E95)+($F$2*F95)+($G$2*G95)+($H$2*H95)+($I$2*I95)+($J$2*J95)+($K$2*K95)+($L$2*L95)+($M$2*M95)+($N$2*N95)+($O$2*O95)+($P$2*P95)+($Q$2*Q95)+($R$2*R95)+($S$2*S95)+($T$2*T95)+($U$2*U95)+($V$2*V95)+($W$2*W95)+($X$2*X95)+($Y$2*Y95)+($Z$2*Z95)+(AA95)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C96" s="18" t="n">
         <v>3101</v>
+      </c>
+      <c r="D96" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB96" s="17" t="n">
+        <f aca="false">($D$2*D96)+($E$2*E96)+($F$2*F96)+($G$2*G96)+($H$2*H96)+($I$2*I96)+($J$2*J96)+($K$2*K96)+($L$2*L96)+($M$2*M96)+($N$2*N96)+($O$2*O96)+($P$2*P96)+($Q$2*Q96)+($R$2*R96)+($S$2*S96)+($T$2*T96)+($U$2*U96)+($V$2*V96)+($W$2*W96)+($X$2*X96)+($Y$2*Y96)+($Z$2*Z96)+(AA96)</f>
+        <v>1300</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="18" t="n">
         <v>3102</v>
       </c>
+      <c r="AB97" s="17" t="n">
+        <f aca="false">($D$2*D97)+($E$2*E97)+($F$2*F97)+($G$2*G97)+($H$2*H97)+($I$2*I97)+($J$2*J97)+($K$2*K97)+($L$2*L97)+($M$2*M97)+($N$2*N97)+($O$2*O97)+($P$2*P97)+($Q$2*Q97)+($R$2*R97)+($S$2*S97)+($T$2*T97)+($U$2*U97)+($V$2*V97)+($W$2*W97)+($X$2*X97)+($Y$2*Y97)+($Z$2*Z97)+(AA97)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="18" t="n">
         <v>3103</v>
       </c>
+      <c r="AB98" s="17" t="n">
+        <f aca="false">($D$2*D98)+($E$2*E98)+($F$2*F98)+($G$2*G98)+($H$2*H98)+($I$2*I98)+($J$2*J98)+($K$2*K98)+($L$2*L98)+($M$2*M98)+($N$2*N98)+($O$2*O98)+($P$2*P98)+($Q$2*Q98)+($R$2*R98)+($S$2*S98)+($T$2*T98)+($U$2*U98)+($V$2*V98)+($W$2*W98)+($X$2*X98)+($Y$2*Y98)+($Z$2*Z98)+(AA98)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="18" t="n">
         <v>3104</v>
+      </c>
+      <c r="AB99" s="17" t="n">
+        <f aca="false">($D$2*D99)+($E$2*E99)+($F$2*F99)+($G$2*G99)+($H$2*H99)+($I$2*I99)+($J$2*J99)+($K$2*K99)+($L$2*L99)+($M$2*M99)+($N$2*N99)+($O$2*O99)+($P$2*P99)+($Q$2*Q99)+($R$2*R99)+($S$2*S99)+($T$2*T99)+($U$2*U99)+($V$2*V99)+($W$2*W99)+($X$2*X99)+($Y$2*Y99)+($Z$2*Z99)+(AA99)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Item Tree Work / Bug Fixes
- Staff of Sorcery
- Superior Int
- fixed bug when two misc items combine in inventory and become null refs
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -863,7 +863,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G95" activeCellId="0" sqref="G95"/>
+      <selection pane="bottomLeft" activeCell="B110" activeCellId="0" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7091,6 +7091,9 @@
       <c r="A110" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="B110" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="C110" s="18" t="n">
         <v>3115</v>
       </c>

</xml_diff>

<commit_message>
[WIP] Item - Circes Staff
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="153">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -473,6 +473,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_rauoskinna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_circes_staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_circes_staff</t>
   </si>
 </sst>
 </file>
@@ -884,10 +890,10 @@
   </sheetPr>
   <dimension ref="A1:AC132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="Z118" activeCellId="0" sqref="Z118"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="AA120" activeCellId="0" sqref="AA120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7283,6 +7289,12 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C119" s="18" t="n">
         <v>3124</v>
       </c>
@@ -7292,12 +7304,36 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C120" s="18" t="n">
         <v>3125</v>
       </c>
+      <c r="D120" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E120" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F120" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="V120" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Y120" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z120" s="1" t="n">
+        <v>1000</v>
+      </c>
       <c r="AB120" s="17" t="n">
         <f aca="false">($D$2*D120)+($E$2*E120)+($F$2*F120)+($G$2*G120)+($H$2*H120)+($I$2*I120)+($J$2*J120)+($K$2*K120)+($L$2*L120)+($M$2*M120)+($N$2*N120)+($O$2*O120)+($P$2*P120)+($Q$2*Q120)+($R$2*R120)+($S$2*S120)+($T$2*T120)+($U$2*U120)+($V$2*V120)+($W$2*W120)+($X$2*X120)+($Y$2*Y120)+($Z$2*Z120)+(AA120)</f>
-        <v>0</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Item - Nemean Lion's Hide
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="155">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_circes_staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_nemean_lions_hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_nemean_lions_hide</t>
   </si>
 </sst>
 </file>
@@ -891,9 +897,9 @@
   <dimension ref="A1:AC132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AA120" activeCellId="0" sqref="AA120"/>
+      <selection pane="bottomLeft" activeCell="S125" activeCellId="0" sqref="S125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7337,6 +7343,12 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C121" s="18" t="n">
         <v>3126</v>
       </c>
@@ -7346,12 +7358,30 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B122" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="C122" s="18" t="n">
         <v>3127</v>
       </c>
+      <c r="F122" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I122" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="J122" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O122" s="1" t="n">
+        <v>50</v>
+      </c>
       <c r="AB122" s="17" t="n">
         <f aca="false">($D$2*D122)+($E$2*E122)+($F$2*F122)+($G$2*G122)+($H$2*H122)+($I$2*I122)+($J$2*J122)+($K$2*K122)+($L$2*L122)+($M$2*M122)+($N$2*N122)+($O$2*O122)+($P$2*P122)+($Q$2*Q122)+($R$2*R122)+($S$2*S122)+($T$2*T122)+($U$2*U122)+($V$2*V122)+($W$2*W122)+($X$2*X122)+($Y$2*Y122)+($Z$2*Z122)+(AA122)</f>
-        <v>0</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Bracer Rework; MK Immortality Fix
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -897,9 +897,9 @@
   <dimension ref="A1:AC132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="S125" activeCellId="0" sqref="S125"/>
+      <selection pane="bottomLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2827,13 +2827,13 @@
         <v>3033</v>
       </c>
       <c r="D28" s="17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" s="17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F28" s="17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G28" s="17" t="n">
         <v>0</v>
@@ -2882,7 +2882,7 @@
       <c r="AA28" s="17"/>
       <c r="AB28" s="17" t="n">
         <f aca="false">($D$2*D28)+($E$2*E28)+($F$2*F28)+($G$2*G28)+($H$2*H28)+($I$2*I28)+($J$2*J28)+($K$2*K28)+($L$2*L28)+($M$2*M28)+($N$2*N28)+($O$2*O28)+($P$2*P28)+($Q$2*Q28)+($R$2*R28)+($S$2*S28)+($T$2*T28)+($U$2*U28)+($V$2*V28)+($W$2*W28)+($X$2*X28)+($Y$2*Y28)+($Z$2*Z28)+(AA28)</f>
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="AC28" s="17" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
[WIP] Item - Armor of Achilles
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="159">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -485,6 +485,18 @@
   </si>
   <si>
     <t xml:space="preserve">item_nemean_lions_hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_greater_attack_speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_greater_attack_speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_armor_of_achilles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_armor_of_achilles</t>
   </si>
 </sst>
 </file>
@@ -897,9 +909,9 @@
   <dimension ref="A1:AC132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+      <selection pane="bottomLeft" activeCell="C126" activeCellId="0" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7385,6 +7397,12 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B123" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C123" s="18" t="n">
         <v>3128</v>
       </c>
@@ -7394,15 +7412,30 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="C124" s="18" t="n">
         <v>3129</v>
       </c>
+      <c r="H124" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="AB124" s="17" t="n">
         <f aca="false">($D$2*D124)+($E$2*E124)+($F$2*F124)+($G$2*G124)+($H$2*H124)+($I$2*I124)+($J$2*J124)+($K$2*K124)+($L$2*L124)+($M$2*M124)+($N$2*N124)+($O$2*O124)+($P$2*P124)+($Q$2*Q124)+($R$2*R124)+($S$2*S124)+($T$2*T124)+($U$2*U124)+($V$2*V124)+($W$2*W124)+($X$2*X124)+($Y$2*Y124)+($Z$2*Z124)+(AA124)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C125" s="18" t="n">
         <v>3130</v>
       </c>
@@ -7412,6 +7445,12 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="C126" s="18" t="n">
         <v>3131</v>
       </c>

</xml_diff>

<commit_message>
Item - Magic Armor
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="161">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_armor_of_achilles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_magic_armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_magic_armor</t>
   </si>
 </sst>
 </file>
@@ -906,12 +912,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC132"/>
+  <dimension ref="A1:AC144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="N126" activeCellId="0" sqref="N126"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D127" activeCellId="0" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7481,6 +7487,12 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B127" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C127" s="18" t="n">
         <v>3132</v>
       </c>
@@ -7490,32 +7502,161 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="C128" s="18" t="n">
+        <v>3133</v>
+      </c>
+      <c r="O128" s="1" t="n">
+        <v>20</v>
+      </c>
       <c r="AB128" s="17" t="n">
         <f aca="false">($D$2*D128)+($E$2*E128)+($F$2*F128)+($G$2*G128)+($H$2*H128)+($I$2*I128)+($J$2*J128)+($K$2*K128)+($L$2*L128)+($M$2*M128)+($N$2*N128)+($O$2*O128)+($P$2*P128)+($Q$2*Q128)+($R$2*R128)+($S$2*S128)+($T$2*T128)+($U$2*U128)+($V$2*V128)+($W$2*W128)+($X$2*X128)+($Y$2*Y128)+($Z$2*Z128)+(AA128)</f>
-        <v>0</v>
+        <v>700</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="18" t="n">
+        <v>3134</v>
+      </c>
       <c r="AB129" s="17" t="n">
         <f aca="false">($D$2*D129)+($E$2*E129)+($F$2*F129)+($G$2*G129)+($H$2*H129)+($I$2*I129)+($J$2*J129)+($K$2*K129)+($L$2*L129)+($M$2*M129)+($N$2*N129)+($O$2*O129)+($P$2*P129)+($Q$2*Q129)+($R$2*R129)+($S$2*S129)+($T$2*T129)+($U$2*U129)+($V$2*V129)+($W$2*W129)+($X$2*X129)+($Y$2*Y129)+($Z$2*Z129)+(AA129)</f>
         <v>0</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="18" t="n">
+        <v>3135</v>
+      </c>
       <c r="AB130" s="17" t="n">
         <f aca="false">($D$2*D130)+($E$2*E130)+($F$2*F130)+($G$2*G130)+($H$2*H130)+($I$2*I130)+($J$2*J130)+($K$2*K130)+($L$2*L130)+($M$2*M130)+($N$2*N130)+($O$2*O130)+($P$2*P130)+($Q$2*Q130)+($R$2*R130)+($S$2*S130)+($T$2*T130)+($U$2*U130)+($V$2*V130)+($W$2*W130)+($X$2*X130)+($Y$2*Y130)+($Z$2*Z130)+(AA130)</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="18" t="n">
+        <v>3136</v>
+      </c>
       <c r="AB131" s="17" t="n">
         <f aca="false">($D$2*D131)+($E$2*E131)+($F$2*F131)+($G$2*G131)+($H$2*H131)+($I$2*I131)+($J$2*J131)+($K$2*K131)+($L$2*L131)+($M$2*M131)+($N$2*N131)+($O$2*O131)+($P$2*P131)+($Q$2*Q131)+($R$2*R131)+($S$2*S131)+($T$2*T131)+($U$2*U131)+($V$2*V131)+($W$2*W131)+($X$2*X131)+($Y$2*Y131)+($Z$2*Z131)+(AA131)</f>
         <v>0</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="18" t="n">
+        <v>3137</v>
+      </c>
       <c r="AB132" s="17" t="n">
         <f aca="false">($D$2*D132)+($E$2*E132)+($F$2*F132)+($G$2*G132)+($H$2*H132)+($I$2*I132)+($J$2*J132)+($K$2*K132)+($L$2*L132)+($M$2*M132)+($N$2*N132)+($O$2*O132)+($P$2*P132)+($Q$2*Q132)+($R$2*R132)+($S$2*S132)+($T$2*T132)+($U$2*U132)+($V$2*V132)+($W$2*W132)+($X$2*X132)+($Y$2*Y132)+($Z$2*Z132)+(AA132)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="18" t="n">
+        <v>3138</v>
+      </c>
+      <c r="AB133" s="17" t="n">
+        <f aca="false">($D$2*D133)+($E$2*E133)+($F$2*F133)+($G$2*G133)+($H$2*H133)+($I$2*I133)+($J$2*J133)+($K$2*K133)+($L$2*L133)+($M$2*M133)+($N$2*N133)+($O$2*O133)+($P$2*P133)+($Q$2*Q133)+($R$2*R133)+($S$2*S133)+($T$2*T133)+($U$2*U133)+($V$2*V133)+($W$2*W133)+($X$2*X133)+($Y$2*Y133)+($Z$2*Z133)+(AA133)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="18" t="n">
+        <v>3139</v>
+      </c>
+      <c r="AB134" s="17" t="n">
+        <f aca="false">($D$2*D134)+($E$2*E134)+($F$2*F134)+($G$2*G134)+($H$2*H134)+($I$2*I134)+($J$2*J134)+($K$2*K134)+($L$2*L134)+($M$2*M134)+($N$2*N134)+($O$2*O134)+($P$2*P134)+($Q$2*Q134)+($R$2*R134)+($S$2*S134)+($T$2*T134)+($U$2*U134)+($V$2*V134)+($W$2*W134)+($X$2*X134)+($Y$2*Y134)+($Z$2*Z134)+(AA134)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="18" t="n">
+        <v>3140</v>
+      </c>
+      <c r="AB135" s="17" t="n">
+        <f aca="false">($D$2*D135)+($E$2*E135)+($F$2*F135)+($G$2*G135)+($H$2*H135)+($I$2*I135)+($J$2*J135)+($K$2*K135)+($L$2*L135)+($M$2*M135)+($N$2*N135)+($O$2*O135)+($P$2*P135)+($Q$2*Q135)+($R$2*R135)+($S$2*S135)+($T$2*T135)+($U$2*U135)+($V$2*V135)+($W$2*W135)+($X$2*X135)+($Y$2*Y135)+($Z$2*Z135)+(AA135)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C136" s="18" t="n">
+        <v>3141</v>
+      </c>
+      <c r="AB136" s="17" t="n">
+        <f aca="false">($D$2*D136)+($E$2*E136)+($F$2*F136)+($G$2*G136)+($H$2*H136)+($I$2*I136)+($J$2*J136)+($K$2*K136)+($L$2*L136)+($M$2*M136)+($N$2*N136)+($O$2*O136)+($P$2*P136)+($Q$2*Q136)+($R$2*R136)+($S$2*S136)+($T$2*T136)+($U$2*U136)+($V$2*V136)+($W$2*W136)+($X$2*X136)+($Y$2*Y136)+($Z$2*Z136)+(AA136)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C137" s="18" t="n">
+        <v>3142</v>
+      </c>
+      <c r="AB137" s="17" t="n">
+        <f aca="false">($D$2*D137)+($E$2*E137)+($F$2*F137)+($G$2*G137)+($H$2*H137)+($I$2*I137)+($J$2*J137)+($K$2*K137)+($L$2*L137)+($M$2*M137)+($N$2*N137)+($O$2*O137)+($P$2*P137)+($Q$2*Q137)+($R$2*R137)+($S$2*S137)+($T$2*T137)+($U$2*U137)+($V$2*V137)+($W$2*W137)+($X$2*X137)+($Y$2*Y137)+($Z$2*Z137)+(AA137)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="18" t="n">
+        <v>3143</v>
+      </c>
+      <c r="AB138" s="17" t="n">
+        <f aca="false">($D$2*D138)+($E$2*E138)+($F$2*F138)+($G$2*G138)+($H$2*H138)+($I$2*I138)+($J$2*J138)+($K$2*K138)+($L$2*L138)+($M$2*M138)+($N$2*N138)+($O$2*O138)+($P$2*P138)+($Q$2*Q138)+($R$2*R138)+($S$2*S138)+($T$2*T138)+($U$2*U138)+($V$2*V138)+($W$2*W138)+($X$2*X138)+($Y$2*Y138)+($Z$2*Z138)+(AA138)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="18" t="n">
+        <v>3144</v>
+      </c>
+      <c r="AB139" s="17" t="n">
+        <f aca="false">($D$2*D139)+($E$2*E139)+($F$2*F139)+($G$2*G139)+($H$2*H139)+($I$2*I139)+($J$2*J139)+($K$2*K139)+($L$2*L139)+($M$2*M139)+($N$2*N139)+($O$2*O139)+($P$2*P139)+($Q$2*Q139)+($R$2*R139)+($S$2*S139)+($T$2*T139)+($U$2*U139)+($V$2*V139)+($W$2*W139)+($X$2*X139)+($Y$2*Y139)+($Z$2*Z139)+(AA139)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="18" t="n">
+        <v>3145</v>
+      </c>
+      <c r="AB140" s="17" t="n">
+        <f aca="false">($D$2*D140)+($E$2*E140)+($F$2*F140)+($G$2*G140)+($H$2*H140)+($I$2*I140)+($J$2*J140)+($K$2*K140)+($L$2*L140)+($M$2*M140)+($N$2*N140)+($O$2*O140)+($P$2*P140)+($Q$2*Q140)+($R$2*R140)+($S$2*S140)+($T$2*T140)+($U$2*U140)+($V$2*V140)+($W$2*W140)+($X$2*X140)+($Y$2*Y140)+($Z$2*Z140)+(AA140)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="18" t="n">
+        <v>3146</v>
+      </c>
+      <c r="AB141" s="17" t="n">
+        <f aca="false">($D$2*D141)+($E$2*E141)+($F$2*F141)+($G$2*G141)+($H$2*H141)+($I$2*I141)+($J$2*J141)+($K$2*K141)+($L$2*L141)+($M$2*M141)+($N$2*N141)+($O$2*O141)+($P$2*P141)+($Q$2*Q141)+($R$2*R141)+($S$2*S141)+($T$2*T141)+($U$2*U141)+($V$2*V141)+($W$2*W141)+($X$2*X141)+($Y$2*Y141)+($Z$2*Z141)+(AA141)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C142" s="18" t="n">
+        <v>3147</v>
+      </c>
+      <c r="AB142" s="17" t="n">
+        <f aca="false">($D$2*D142)+($E$2*E142)+($F$2*F142)+($G$2*G142)+($H$2*H142)+($I$2*I142)+($J$2*J142)+($K$2*K142)+($L$2*L142)+($M$2*M142)+($N$2*N142)+($O$2*O142)+($P$2*P142)+($Q$2*Q142)+($R$2*R142)+($S$2*S142)+($T$2*T142)+($U$2*U142)+($V$2*V142)+($W$2*W142)+($X$2*X142)+($Y$2*Y142)+($Z$2*Z142)+(AA142)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C143" s="18" t="n">
+        <v>3148</v>
+      </c>
+      <c r="AB143" s="17" t="n">
+        <f aca="false">($D$2*D143)+($E$2*E143)+($F$2*F143)+($G$2*G143)+($H$2*H143)+($I$2*I143)+($J$2*J143)+($K$2*K143)+($L$2*L143)+($M$2*M143)+($N$2*N143)+($O$2*O143)+($P$2*P143)+($Q$2*Q143)+($R$2*R143)+($S$2*S143)+($T$2*T143)+($U$2*U143)+($V$2*V143)+($W$2*W143)+($X$2*X143)+($Y$2*Y143)+($Z$2*Z143)+(AA143)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB144" s="17" t="n">
+        <f aca="false">($D$2*D144)+($E$2*E144)+($F$2*F144)+($G$2*G144)+($H$2*H144)+($I$2*I144)+($J$2*J144)+($K$2*K144)+($L$2*L144)+($M$2*M144)+($N$2*N144)+($O$2*O144)+($P$2*P144)+($Q$2*Q144)+($R$2*R144)+($S$2*S144)+($T$2*T144)+($U$2*U144)+($V$2*V144)+($W$2*W144)+($X$2*X144)+($Y$2*Y144)+($Z$2*Z144)+(AA144)</f>
         <v>0</v>
       </c>
     </row>
@@ -7524,7 +7665,7 @@
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="A3:AC3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C135:C1048576 C3:C127 D3:AC1048576 A3:B1048576">
+  <conditionalFormatting sqref="A3:AC1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
[WIP] Item - Adder Stone
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="169">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_superior_hp_regen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_adder_stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_adder_stone</t>
   </si>
 </sst>
 </file>
@@ -932,10 +938,10 @@
   </sheetPr>
   <dimension ref="A1:AC144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C131" activeCellId="0" sqref="C131"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="AA136" activeCellId="0" sqref="AA136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7637,6 +7643,12 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C135" s="18" t="n">
         <v>3140</v>
       </c>
@@ -7646,12 +7658,27 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="C136" s="18" t="n">
         <v>3141</v>
       </c>
+      <c r="O136" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="T136" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="V136" s="1" t="n">
+        <v>1.3</v>
+      </c>
       <c r="AB136" s="17" t="n">
         <f aca="false">($D$2*D136)+($E$2*E136)+($F$2*F136)+($G$2*G136)+($H$2*H136)+($I$2*I136)+($J$2*J136)+($K$2*K136)+($L$2*L136)+($M$2*M136)+($N$2*N136)+($O$2*O136)+($P$2*P136)+($Q$2*Q136)+($R$2*R136)+($S$2*S136)+($T$2*T136)+($U$2*U136)+($V$2*V136)+($W$2*W136)+($X$2*X136)+($Y$2*Y136)+($Z$2*Z136)+(AA136)</f>
-        <v>0</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Ring of Dispel
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="171">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_adder_stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_ring_of_dispel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_ring_of_dispel</t>
   </si>
 </sst>
 </file>
@@ -939,9 +945,9 @@
   <dimension ref="A1:AC144"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AA136" activeCellId="0" sqref="AA136"/>
+      <selection pane="bottomLeft" activeCell="K134" activeCellId="0" sqref="K134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7682,6 +7688,12 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C137" s="18" t="n">
         <v>3142</v>
       </c>
@@ -7691,12 +7703,33 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="C138" s="18" t="n">
         <v>3143</v>
       </c>
+      <c r="J138" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O138" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="T138" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="V138" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Y138" s="1" t="n">
+        <v>100</v>
+      </c>
       <c r="AB138" s="17" t="n">
         <f aca="false">($D$2*D138)+($E$2*E138)+($F$2*F138)+($G$2*G138)+($H$2*H138)+($I$2*I138)+($J$2*J138)+($K$2*K138)+($L$2*L138)+($M$2*M138)+($N$2*N138)+($O$2*O138)+($P$2*P138)+($Q$2*Q138)+($R$2*R138)+($S$2*S138)+($T$2*T138)+($U$2*U138)+($V$2*V138)+($W$2*W138)+($X$2*X138)+($Y$2*Y138)+($Z$2*Z138)+(AA138)</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Jarngreipr
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_ring_of_dispel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_jarngreipr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_jarngreipr</t>
   </si>
 </sst>
 </file>
@@ -944,10 +950,10 @@
   </sheetPr>
   <dimension ref="A1:AC144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K134" activeCellId="0" sqref="K134"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7733,6 +7739,12 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C139" s="18" t="n">
         <v>3144</v>
       </c>
@@ -7742,12 +7754,27 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>3</v>
+      </c>
       <c r="C140" s="18" t="n">
         <v>3145</v>
       </c>
+      <c r="F140" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J140" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="V140" s="1" t="n">
+        <v>2.5</v>
+      </c>
       <c r="AB140" s="17" t="n">
         <f aca="false">($D$2*D140)+($E$2*E140)+($F$2*F140)+($G$2*G140)+($H$2*H140)+($I$2*I140)+($J$2*J140)+($K$2*K140)+($L$2*L140)+($M$2*M140)+($N$2*N140)+($O$2*O140)+($P$2*P140)+($Q$2*Q140)+($R$2*R140)+($S$2*S140)+($T$2*T140)+($U$2*U140)+($V$2*V140)+($W$2*W140)+($X$2*X140)+($Y$2*Y140)+($Z$2*Z140)+(AA140)</f>
-        <v>0</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Lifesteal
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="174">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t xml:space="preserve">item_jarngreipr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_avalore_lifesteal</t>
   </si>
 </sst>
 </file>
@@ -950,10 +953,10 @@
   </sheetPr>
   <dimension ref="A1:AC144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="R137" activeCellId="0" sqref="R137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1044,7 +1047,7 @@
         <v>100</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L2" s="5" t="n">
         <v>12</v>
@@ -7778,12 +7781,21 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B141" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="C141" s="18" t="n">
         <v>3146</v>
       </c>
+      <c r="K141" s="1" t="n">
+        <v>15</v>
+      </c>
       <c r="AB141" s="17" t="n">
         <f aca="false">($D$2*D141)+($E$2*E141)+($F$2*F141)+($G$2*G141)+($H$2*H141)+($I$2*I141)+($J$2*J141)+($K$2*K141)+($L$2*L141)+($M$2*M141)+($N$2*N141)+($O$2*O141)+($P$2*P141)+($Q$2*Q141)+($R$2*R141)+($S$2*S141)+($T$2*T141)+($U$2*U141)+($V$2*V141)+($W$2*W141)+($X$2*X141)+($Y$2*Y141)+($Z$2*Z141)+(AA141)</f>
-        <v>0</v>
+        <v>750</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Hatchet
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -542,6 +542,9 @@
   </si>
   <si>
     <t xml:space="preserve">item_avalore_lifesteal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_hatchet</t>
   </si>
 </sst>
 </file>
@@ -956,7 +959,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="R137" activeCellId="0" sqref="R137"/>
+      <selection pane="bottomLeft" activeCell="I142" activeCellId="0" sqref="I142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7799,12 +7802,21 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B142" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C142" s="18" t="n">
         <v>3147</v>
       </c>
+      <c r="Z142" s="1" t="n">
+        <v>150</v>
+      </c>
       <c r="AB142" s="17" t="n">
         <f aca="false">($D$2*D142)+($E$2*E142)+($F$2*F142)+($G$2*G142)+($H$2*H142)+($I$2*I142)+($J$2*J142)+($K$2*K142)+($L$2*L142)+($M$2*M142)+($N$2*N142)+($O$2*O142)+($P$2*P142)+($Q$2*Q142)+($R$2*R142)+($S$2*S142)+($T$2*T142)+($U$2*U142)+($V$2*V142)+($W$2*W142)+($X$2*X142)+($Y$2*Y142)+($Z$2*Z142)+(AA142)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Paul Bunyan's Axe
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="177">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_hatchet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_paul_bunyans_axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_paul_bunyans_axe</t>
   </si>
 </sst>
 </file>
@@ -954,12 +960,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC144"/>
+  <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I142" activeCellId="0" sqref="I142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A144" activeCellId="0" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7820,6 +7826,12 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B143" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C143" s="18" t="n">
         <v>3148</v>
       </c>
@@ -7829,9 +7841,125 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C144" s="18" t="n">
+        <v>3149</v>
+      </c>
+      <c r="F144" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I144" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="T144" s="1" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="Z144" s="1" t="n">
+        <v>150</v>
+      </c>
       <c r="AB144" s="17" t="n">
         <f aca="false">($D$2*D144)+($E$2*E144)+($F$2*F144)+($G$2*G144)+($H$2*H144)+($I$2*I144)+($J$2*J144)+($K$2*K144)+($L$2*L144)+($M$2*M144)+($N$2*N144)+($O$2*O144)+($P$2*P144)+($Q$2*Q144)+($R$2*R144)+($S$2*S144)+($T$2*T144)+($U$2*U144)+($V$2*V144)+($W$2*W144)+($X$2*X144)+($Y$2*Y144)+($Z$2*Z144)+(AA144)</f>
-        <v>0</v>
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C145" s="18" t="n">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C146" s="18" t="n">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C147" s="18" t="n">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C148" s="18" t="n">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C149" s="18" t="n">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="18" t="n">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="18" t="n">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="18" t="n">
+        <v>3157</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C153" s="18" t="n">
+        <v>3158</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C154" s="18" t="n">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C155" s="18" t="n">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C156" s="18" t="n">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C157" s="18" t="n">
+        <v>3162</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="18" t="n">
+        <v>3163</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="18" t="n">
+        <v>3164</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="18" t="n">
+        <v>3165</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="18" t="n">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C162" s="18" t="n">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C163" s="18" t="n">
+        <v>3168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Item - Recurve Bow
- Added a better build-up item (and binds to the slot) for Apollo's Bow
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="183">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -563,6 +563,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_recurve_bow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recurve_bow</t>
   </si>
 </sst>
 </file>
@@ -974,10 +980,10 @@
   </sheetPr>
   <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AB146" activeCellId="0" sqref="AB146"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E146" activeCellId="0" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7905,7 +7911,7 @@
         <v>3151</v>
       </c>
       <c r="D146" s="1" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H146" s="1" t="n">
         <v>60</v>
@@ -7915,7 +7921,7 @@
       </c>
       <c r="AB146" s="17" t="n">
         <f aca="false">($D$2*D146)+($E$2*E146)+($F$2*F146)+($G$2*G146)+($H$2*H146)+($I$2*I146)+($J$2*J146)+($K$2*K146)+($L$2*L146)+($M$2*M146)+($N$2*N146)+($O$2*O146)+($P$2*P146)+($Q$2*Q146)+($R$2*R146)+($S$2*S146)+($T$2*T146)+($U$2*U146)+($V$2*V146)+($W$2*W146)+($X$2*X146)+($Y$2*Y146)+($Z$2*Z146)+(AA146)</f>
-        <v>2800</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7955,6 +7961,12 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B149" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C149" s="18" t="n">
         <v>3154</v>
       </c>
@@ -7964,12 +7976,24 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C150" s="18" t="n">
         <v>3155</v>
       </c>
+      <c r="D150" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H150" s="1" t="n">
+        <v>15</v>
+      </c>
       <c r="AB150" s="17" t="n">
         <f aca="false">($D$2*D150)+($E$2*E150)+($F$2*F150)+($G$2*G150)+($H$2*H150)+($I$2*I150)+($J$2*J150)+($K$2*K150)+($L$2*L150)+($M$2*M150)+($N$2*N150)+($O$2*O150)+($P$2*P150)+($Q$2*Q150)+($R$2*R150)+($S$2*S150)+($T$2*T150)+($U$2*U150)+($V$2*V150)+($W$2*W150)+($X$2*X150)+($Y$2*Y150)+($Z$2*Z150)+(AA150)</f>
-        <v>0</v>
+        <v>800</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Sacis Cap
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="189">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_ars_goetia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_sacis_cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_sacis_cap</t>
   </si>
 </sst>
 </file>
@@ -992,10 +998,10 @@
   </sheetPr>
   <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="N156" activeCellId="0" sqref="N156"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A156" activeCellId="0" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8081,6 +8087,12 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B155" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C155" s="18" t="n">
         <v>3160</v>
       </c>
@@ -8090,12 +8102,21 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="C156" s="18" t="n">
         <v>3161</v>
       </c>
+      <c r="Z156" s="1" t="n">
+        <v>2200</v>
+      </c>
       <c r="AB156" s="17" t="n">
         <f aca="false">($D$2*D156)+($E$2*E156)+($F$2*F156)+($G$2*G156)+($H$2*H156)+($I$2*I156)+($J$2*J156)+($K$2*K156)+($L$2*L156)+($M$2*M156)+($N$2*N156)+($O$2*O156)+($P$2*P156)+($Q$2*Q156)+($R$2*R156)+($S$2*S156)+($T$2*T156)+($U$2*U156)+($V$2*V156)+($W$2*W156)+($X$2*X156)+($Y$2*Y156)+($Z$2*Z156)+(AA156)</f>
-        <v>0</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Gungnir
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -587,6 +587,18 @@
   </si>
   <si>
     <t xml:space="preserve">item_sacis_cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_gungnir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_gungnir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_spear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_spear</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1013,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A156" activeCellId="0" sqref="A156"/>
+      <selection pane="bottomLeft" activeCell="I158" activeCellId="0" sqref="I158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8120,6 +8132,12 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B157" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C157" s="18" t="n">
         <v>3162</v>
       </c>
@@ -8129,15 +8147,36 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B158" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C158" s="18" t="n">
         <v>3163</v>
       </c>
+      <c r="H158" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="I158" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="S158" s="1" t="n">
+        <v>150</v>
+      </c>
       <c r="AB158" s="17" t="n">
         <f aca="false">($D$2*D158)+($E$2*E158)+($F$2*F158)+($G$2*G158)+($H$2*H158)+($I$2*I158)+($J$2*J158)+($K$2*K158)+($L$2*L158)+($M$2*M158)+($N$2*N158)+($O$2*O158)+($P$2*P158)+($Q$2*Q158)+($R$2*R158)+($S$2*S158)+($T$2*T158)+($U$2*U158)+($V$2*V158)+($W$2*W158)+($X$2*X158)+($Y$2*Y158)+($Z$2*Z158)+(AA158)</f>
-        <v>0</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B159" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C159" s="18" t="n">
         <v>3164</v>
       </c>
@@ -8147,12 +8186,24 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B160" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C160" s="18" t="n">
         <v>3165</v>
       </c>
+      <c r="H160" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I160" s="1" t="n">
+        <v>15</v>
+      </c>
       <c r="AB160" s="17" t="n">
         <f aca="false">($D$2*D160)+($E$2*E160)+($F$2*F160)+($G$2*G160)+($H$2*H160)+($I$2*I160)+($J$2*J160)+($K$2*K160)+($L$2*L160)+($M$2*M160)+($N$2*N160)+($O$2*O160)+($P$2*P160)+($Q$2*Q160)+($R$2*R160)+($S$2*S160)+($T$2*T160)+($U$2*U160)+($V$2*V160)+($W$2*W160)+($X$2*X160)+($Y$2*Y160)+($Z$2*Z160)+(AA160)</f>
-        <v>0</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Items - Spear, Gungnir
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -1010,10 +1010,10 @@
   </sheetPr>
   <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I158" activeCellId="0" sqref="I158"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="P160" activeCellId="0" sqref="P160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[WIP] Item - Gleipnir
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="196">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -599,6 +599,15 @@
   </si>
   <si>
     <t xml:space="preserve">item_spear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_vitality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_gleipnir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_gleipnir</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1019,10 @@
   </sheetPr>
   <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="P160" activeCellId="0" sqref="P160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="W163" activeCellId="0" sqref="W163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8207,22 +8216,69 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B161" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="C161" s="18" t="n">
         <v>3166</v>
       </c>
+      <c r="X161" s="1" t="n">
+        <v>100</v>
+      </c>
       <c r="AB161" s="17" t="n">
         <f aca="false">($D$2*D161)+($E$2*E161)+($F$2*F161)+($G$2*G161)+($H$2*H161)+($I$2*I161)+($J$2*J161)+($K$2*K161)+($L$2*L161)+($M$2*M161)+($N$2*N161)+($O$2*O161)+($P$2*P161)+($Q$2*Q161)+($R$2*R161)+($S$2*S161)+($T$2*T161)+($U$2*U161)+($V$2*V161)+($W$2*W161)+($X$2*X161)+($Y$2*Y161)+($Z$2*Z161)+(AA161)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B162" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C162" s="18" t="n">
         <v>3167</v>
       </c>
+      <c r="AB162" s="17" t="n">
+        <f aca="false">($D$2*D162)+($E$2*E162)+($F$2*F162)+($G$2*G162)+($H$2*H162)+($I$2*I162)+($J$2*J162)+($K$2*K162)+($L$2*L162)+($M$2*M162)+($N$2*N162)+($O$2*O162)+($P$2*P162)+($Q$2*Q162)+($R$2*R162)+($S$2*S162)+($T$2*T162)+($U$2*U162)+($V$2*V162)+($W$2*W162)+($X$2*X162)+($Y$2*Y162)+($Z$2*Z162)+(AA162)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B163" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C163" s="18" t="n">
         <v>3168</v>
+      </c>
+      <c r="D163" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E163" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="F163" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="T163" s="1" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V163" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="X163" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB163" s="17" t="n">
+        <f aca="false">($D$2*D163)+($E$2*E163)+($F$2*F163)+($G$2*G163)+($H$2*H163)+($I$2*I163)+($J$2*J163)+($K$2*K163)+($L$2*L163)+($M$2*M163)+($N$2*N163)+($O$2*O163)+($P$2*P163)+($Q$2*Q163)+($R$2*R163)+($S$2*S163)+($T$2*T163)+($U$2*U163)+($V$2*V163)+($W$2*W163)+($X$2*X163)+($Y$2*Y163)+($Z$2*Z163)+(AA163)</f>
+        <v>3715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WIP] Item - Chrysaor
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="199">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -608,6 +608,15 @@
   </si>
   <si>
     <t xml:space="preserve">item_gleipnir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_adamant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_chrysaor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_chrysaor</t>
   </si>
 </sst>
 </file>
@@ -823,7 +832,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -918,6 +927,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1017,12 +1030,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC163"/>
+  <dimension ref="A1:AC180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="W163" activeCellId="0" sqref="W163"/>
+      <selection pane="bottomLeft" activeCell="E180" activeCellId="0" sqref="E180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8281,12 +8294,162 @@
         <v>3715</v>
       </c>
     </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B164" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="C164" s="18" t="n">
+        <v>3169</v>
+      </c>
+      <c r="Z164" s="24" t="n">
+        <v>300</v>
+      </c>
+      <c r="AB164" s="17" t="n">
+        <f aca="false">($D$2*D164)+($E$2*E164)+($F$2*F164)+($G$2*G164)+($H$2*H164)+($I$2*I164)+($J$2*J164)+($K$2*K164)+($L$2*L164)+($M$2*M164)+($N$2*N164)+($O$2*O164)+($P$2*P164)+($Q$2*Q164)+($R$2*R164)+($S$2*S164)+($T$2*T164)+($U$2*U164)+($V$2*V164)+($W$2*W164)+($X$2*X164)+($Y$2*Y164)+($Z$2*Z164)+(AA164)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B165" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C165" s="18" t="n">
+        <v>3170</v>
+      </c>
+      <c r="AB165" s="17" t="n">
+        <f aca="false">($D$2*D165)+($E$2*E165)+($F$2*F165)+($G$2*G165)+($H$2*H165)+($I$2*I165)+($J$2*J165)+($K$2*K165)+($L$2*L165)+($M$2*M165)+($N$2*N165)+($O$2*O165)+($P$2*P165)+($Q$2*Q165)+($R$2*R165)+($S$2*S165)+($T$2*T165)+($U$2*U165)+($V$2*V165)+($W$2*W165)+($X$2*X165)+($Y$2*Y165)+($Z$2*Z165)+(AA165)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B166" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C166" s="18" t="n">
+        <v>3171</v>
+      </c>
+      <c r="AB166" s="17" t="n">
+        <f aca="false">($D$2*D166)+($E$2*E166)+($F$2*F166)+($G$2*G166)+($H$2*H166)+($I$2*I166)+($J$2*J166)+($K$2*K166)+($L$2*L166)+($M$2*M166)+($N$2*N166)+($O$2*O166)+($P$2*P166)+($Q$2*Q166)+($R$2*R166)+($S$2*S166)+($T$2*T166)+($U$2*U166)+($V$2*V166)+($W$2*W166)+($X$2*X166)+($Y$2*Y166)+($Z$2*Z166)+(AA166)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="18" t="n">
+        <v>3172</v>
+      </c>
+      <c r="AB167" s="17" t="n">
+        <f aca="false">($D$2*D167)+($E$2*E167)+($F$2*F167)+($G$2*G167)+($H$2*H167)+($I$2*I167)+($J$2*J167)+($K$2*K167)+($L$2*L167)+($M$2*M167)+($N$2*N167)+($O$2*O167)+($P$2*P167)+($Q$2*Q167)+($R$2*R167)+($S$2*S167)+($T$2*T167)+($U$2*U167)+($V$2*V167)+($W$2*W167)+($X$2*X167)+($Y$2*Y167)+($Z$2*Z167)+(AA167)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C168" s="18" t="n">
+        <v>3173</v>
+      </c>
+      <c r="AB168" s="17" t="n">
+        <f aca="false">($D$2*D168)+($E$2*E168)+($F$2*F168)+($G$2*G168)+($H$2*H168)+($I$2*I168)+($J$2*J168)+($K$2*K168)+($L$2*L168)+($M$2*M168)+($N$2*N168)+($O$2*O168)+($P$2*P168)+($Q$2*Q168)+($R$2*R168)+($S$2*S168)+($T$2*T168)+($U$2*U168)+($V$2*V168)+($W$2*W168)+($X$2*X168)+($Y$2*Y168)+($Z$2*Z168)+(AA168)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C169" s="18" t="n">
+        <v>3174</v>
+      </c>
+      <c r="AB169" s="17" t="n">
+        <f aca="false">($D$2*D169)+($E$2*E169)+($F$2*F169)+($G$2*G169)+($H$2*H169)+($I$2*I169)+($J$2*J169)+($K$2*K169)+($L$2*L169)+($M$2*M169)+($N$2*N169)+($O$2*O169)+($P$2*P169)+($Q$2*Q169)+($R$2*R169)+($S$2*S169)+($T$2*T169)+($U$2*U169)+($V$2*V169)+($W$2*W169)+($X$2*X169)+($Y$2*Y169)+($Z$2*Z169)+(AA169)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="18" t="n">
+        <v>3175</v>
+      </c>
+      <c r="AB170" s="17" t="n">
+        <f aca="false">($D$2*D170)+($E$2*E170)+($F$2*F170)+($G$2*G170)+($H$2*H170)+($I$2*I170)+($J$2*J170)+($K$2*K170)+($L$2*L170)+($M$2*M170)+($N$2*N170)+($O$2*O170)+($P$2*P170)+($Q$2*Q170)+($R$2*R170)+($S$2*S170)+($T$2*T170)+($U$2*U170)+($V$2*V170)+($W$2*W170)+($X$2*X170)+($Y$2*Y170)+($Z$2*Z170)+(AA170)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="18" t="n">
+        <v>3176</v>
+      </c>
+      <c r="AB171" s="17" t="n">
+        <f aca="false">($D$2*D171)+($E$2*E171)+($F$2*F171)+($G$2*G171)+($H$2*H171)+($I$2*I171)+($J$2*J171)+($K$2*K171)+($L$2*L171)+($M$2*M171)+($N$2*N171)+($O$2*O171)+($P$2*P171)+($Q$2*Q171)+($R$2*R171)+($S$2*S171)+($T$2*T171)+($U$2*U171)+($V$2*V171)+($W$2*W171)+($X$2*X171)+($Y$2*Y171)+($Z$2*Z171)+(AA171)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C172" s="18" t="n">
+        <v>3177</v>
+      </c>
+      <c r="AB172" s="17" t="n">
+        <f aca="false">($D$2*D172)+($E$2*E172)+($F$2*F172)+($G$2*G172)+($H$2*H172)+($I$2*I172)+($J$2*J172)+($K$2*K172)+($L$2*L172)+($M$2*M172)+($N$2*N172)+($O$2*O172)+($P$2*P172)+($Q$2*Q172)+($R$2*R172)+($S$2*S172)+($T$2*T172)+($U$2*U172)+($V$2*V172)+($W$2*W172)+($X$2*X172)+($Y$2*Y172)+($Z$2*Z172)+(AA172)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="18" t="n">
+        <v>3178</v>
+      </c>
+      <c r="AB173" s="17" t="n">
+        <f aca="false">($D$2*D173)+($E$2*E173)+($F$2*F173)+($G$2*G173)+($H$2*H173)+($I$2*I173)+($J$2*J173)+($K$2*K173)+($L$2*L173)+($M$2*M173)+($N$2*N173)+($O$2*O173)+($P$2*P173)+($Q$2*Q173)+($R$2*R173)+($S$2*S173)+($T$2*T173)+($U$2*U173)+($V$2*V173)+($W$2*W173)+($X$2*X173)+($Y$2*Y173)+($Z$2*Z173)+(AA173)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C174" s="18" t="n">
+        <v>3179</v>
+      </c>
+      <c r="AB174" s="17" t="n">
+        <f aca="false">($D$2*D174)+($E$2*E174)+($F$2*F174)+($G$2*G174)+($H$2*H174)+($I$2*I174)+($J$2*J174)+($K$2*K174)+($L$2*L174)+($M$2*M174)+($N$2*N174)+($O$2*O174)+($P$2*P174)+($Q$2*Q174)+($R$2*R174)+($S$2*S174)+($T$2*T174)+($U$2*U174)+($V$2*V174)+($W$2*W174)+($X$2*X174)+($Y$2*Y174)+($Z$2*Z174)+(AA174)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C175" s="18" t="n">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C176" s="18" t="n">
+        <v>3181</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C177" s="18" t="n">
+        <v>3182</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C178" s="18" t="n">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C179" s="18" t="n">
+        <v>3184</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C180" s="18" t="n">
+        <v>3185</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="A3:AC3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:AC1048576">
+  <conditionalFormatting sqref="A3:AC163 A175:AC1048576 A164:Y164 AB164:AC174 A165:AA174 AA164">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
[WIP] Item - Helm
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="202">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -623,6 +623,9 @@
   </si>
   <si>
     <t xml:space="preserve">item_avalore_broadsword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_helm</t>
   </si>
 </sst>
 </file>
@@ -1039,9 +1042,9 @@
   <dimension ref="A1:AC180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A168" activeCellId="0" sqref="168:168"/>
+      <selection pane="bottomLeft" activeCell="G169" activeCellId="0" sqref="169:169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8388,12 +8391,27 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B169" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="C169" s="18" t="n">
         <v>3174</v>
       </c>
+      <c r="E169" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H169" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="J169" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="AB169" s="17" t="n">
         <f aca="false">($D$2*D169)+($E$2*E169)+($F$2*F169)+($G$2*G169)+($H$2*H169)+($I$2*I169)+($J$2*J169)+($K$2*K169)+($L$2*L169)+($M$2*M169)+($N$2*N169)+($O$2*O169)+($P$2*P169)+($Q$2*Q169)+($R$2*R169)+($S$2*S169)+($T$2*T169)+($U$2*U169)+($V$2*V169)+($W$2*W169)+($X$2*X169)+($Y$2*Y169)+($Z$2*Z169)+(AA169)</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Helm of Hades
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_helm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_helm_of_hades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_helm_of_hades</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1050,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G169" activeCellId="0" sqref="169:169"/>
+      <selection pane="bottomLeft" activeCell="K171" activeCellId="0" sqref="K171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8415,6 +8421,12 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B170" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C170" s="18" t="n">
         <v>3175</v>
       </c>
@@ -8424,12 +8436,27 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B171" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="C171" s="18" t="n">
         <v>3176</v>
       </c>
+      <c r="E171" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H171" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="J171" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="AB171" s="17" t="n">
         <f aca="false">($D$2*D171)+($E$2*E171)+($F$2*F171)+($G$2*G171)+($H$2*H171)+($I$2*I171)+($J$2*J171)+($K$2*K171)+($L$2*L171)+($M$2*M171)+($N$2*N171)+($O$2*O171)+($P$2*P171)+($Q$2*Q171)+($R$2*R171)+($S$2*S171)+($T$2*T171)+($U$2*U171)+($V$2*V171)+($W$2*W171)+($X$2*X171)+($Y$2*Y171)+($Z$2*Z171)+(AA171)</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Item - Helm of Hades
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -1048,9 +1048,9 @@
   <dimension ref="A1:AC180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K171" activeCellId="0" sqref="K171"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="32:32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8449,14 +8449,14 @@
         <v>6</v>
       </c>
       <c r="H171" s="1" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J171" s="1" t="n">
         <v>4</v>
       </c>
       <c r="AB171" s="17" t="n">
         <f aca="false">($D$2*D171)+($E$2*E171)+($F$2*F171)+($G$2*G171)+($H$2*H171)+($I$2*I171)+($J$2*J171)+($K$2*K171)+($L$2*L171)+($M$2*M171)+($N$2*N171)+($O$2*O171)+($P$2*P171)+($Q$2*Q171)+($R$2*R171)+($S$2*S171)+($T$2*T171)+($U$2*U171)+($V$2*V171)+($W$2*W171)+($X$2*X171)+($Y$2*Y171)+($Z$2*Z171)+(AA171)</f>
-        <v>1100</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Ring of Gyges
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="206">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_helm_of_hades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_ring_of_gyges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_ring_of_gyges</t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1050,7 +1056,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="32:32"/>
+      <selection pane="bottomLeft" activeCell="M173" activeCellId="0" sqref="M173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8460,6 +8466,12 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B172" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C172" s="18" t="n">
         <v>3177</v>
       </c>
@@ -8469,12 +8481,24 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B173" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="C173" s="18" t="n">
         <v>3178</v>
       </c>
+      <c r="E173" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I173" s="1" t="n">
+        <v>10</v>
+      </c>
       <c r="AB173" s="17" t="n">
         <f aca="false">($D$2*D173)+($E$2*E173)+($F$2*F173)+($G$2*G173)+($H$2*H173)+($I$2*I173)+($J$2*J173)+($K$2*K173)+($L$2*L173)+($M$2*M173)+($N$2*N173)+($O$2*O173)+($P$2*P173)+($Q$2*Q173)+($R$2*R173)+($S$2*S173)+($T$2*T173)+($U$2*U173)+($V$2*V173)+($W$2*W173)+($X$2*X173)+($Y$2*Y173)+($Z$2*Z173)+(AA173)</f>
-        <v>0</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Item - Mantle of Invisibility
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="208">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -638,6 +638,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_ring_of_gyges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_mantle_of_invisibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_mantle_of_invisibility</t>
   </si>
 </sst>
 </file>
@@ -1054,9 +1060,9 @@
   <dimension ref="A1:AC180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M173" activeCellId="0" sqref="M173"/>
+      <selection pane="bottomLeft" activeCell="C175" activeCellId="0" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8502,6 +8508,12 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B174" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C174" s="18" t="n">
         <v>3179</v>
       </c>
@@ -8511,6 +8523,12 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B175" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="C175" s="18" t="n">
         <v>3180</v>
       </c>

</xml_diff>

<commit_message>
[WIP] Item - Tarnkappe
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="210">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -644,6 +644,12 @@
   </si>
   <si>
     <t xml:space="preserve">item_mantle_of_invisibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_tarnkappe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_tarnkappe</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1068,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C175" activeCellId="0" sqref="C175"/>
+      <selection pane="bottomLeft" activeCell="L177" activeCellId="0" sqref="L177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8532,15 +8538,60 @@
       <c r="C175" s="18" t="n">
         <v>3180</v>
       </c>
+      <c r="D175" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E175" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F175" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G175" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I175" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="J175" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B176" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C176" s="18" t="n">
         <v>3181</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B177" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="C177" s="18" t="n">
         <v>3182</v>
+      </c>
+      <c r="D177" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E177" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F177" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G177" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I177" s="1" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[WIP] Guandao Build up
</commit_message>
<xml_diff>
--- a/balancing/item_balance.xlsx
+++ b/balancing/item_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="223">
   <si>
     <t xml:space="preserve">TODO: Factor in slot efficiency, how many builds use it, time in the game you'd get it, auras, some sort of "ability" cost, base shop vs. secret</t>
   </si>
@@ -677,6 +677,18 @@
   </si>
   <si>
     <t xml:space="preserve">item_frost_fair_blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_bo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_glaive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_recipe_guandao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_guandao</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1111,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C186" activeCellId="0" sqref="C186"/>
+      <selection pane="bottomLeft" activeCell="U190" activeCellId="0" sqref="U190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8803,31 +8815,67 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B187" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C187" s="19" t="n">
         <v>3192</v>
       </c>
+      <c r="S187" s="1" t="n">
+        <v>150</v>
+      </c>
       <c r="AB187" s="18" t="n">
         <f aca="false">($D$2*D187)+($E$2*E187)+($F$2*F187)+($G$2*G187)+($H$2*H187)+($I$2*I187)+($J$2*J187)+($K$2*K187)+($L$2*L187)+($M$2*M187)+($N$2*N187)+($O$2*O187)+($P$2*P187)+($Q$2*Q187)+($R$2*R187)+($S$2*S187)+($T$2*T187)+($U$2*U187)+($V$2*V187)+($W$2*W187)+($X$2*X187)+($Y$2*Y187)+($Z$2*Z187)+(AA187)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B188" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="C188" s="19" t="n">
         <v>3193</v>
       </c>
+      <c r="M188" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="AB188" s="18" t="n">
         <f aca="false">($D$2*D188)+($E$2*E188)+($F$2*F188)+($G$2*G188)+($H$2*H188)+($I$2*I188)+($J$2*J188)+($K$2*K188)+($L$2*L188)+($M$2*M188)+($N$2*N188)+($O$2*O188)+($P$2*P188)+($Q$2*Q188)+($R$2*R188)+($S$2*S188)+($T$2*T188)+($U$2*U188)+($V$2*V188)+($W$2*W188)+($X$2*X188)+($Y$2*Y188)+($Z$2*Z188)+(AA188)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B189" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="C189" s="19" t="n">
         <v>3194</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B190" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="C190" s="19" t="n">
         <v>3195</v>
+      </c>
+      <c r="M190" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S190" s="1" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>